<commit_message>
Added obs data for rainout shelter
</commit_message>
<xml_diff>
--- a/Prototypes/Peanut/Observed.xlsx
+++ b/Prototypes/Peanut/Observed.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Peanut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9260AE61-588C-44FC-80FE-438D339629BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2994BE0-B9F7-4B51-A829-AC301B19BD0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="11136" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="11136" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="14" r:id="rId1"/>
+    <sheet name="Rainout" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$CP$373</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>SimulationName</t>
   </si>
@@ -122,6 +123,21 @@
   <si>
     <t>Peanut.SowingDate</t>
   </si>
+  <si>
+    <t>DAS</t>
+  </si>
+  <si>
+    <t>Pod</t>
+  </si>
+  <si>
+    <t>Biom</t>
+  </si>
+  <si>
+    <t>RainOutSowDec18</t>
+  </si>
+  <si>
+    <t>Stover</t>
+  </si>
 </sst>
 </file>
 
@@ -191,7 +207,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -219,6 +235,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,6 +253,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>483870</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A17DE58C-7D0E-474E-862B-4176ABCE9E35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5215890" y="914400"/>
+          <a:ext cx="2404110" cy="1592580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP373"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -902,36 +985,106 @@
       </c>
     </row>
     <row r="11" spans="1:94" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1">
+        <v>32895</v>
+      </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="1">
+        <v>32860</v>
+      </c>
+      <c r="E11" s="17">
+        <v>35</v>
+      </c>
       <c r="F11" s="1"/>
+      <c r="I11">
+        <v>0.65</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>68.141720896601512</v>
+      </c>
     </row>
     <row r="12" spans="1:94" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1">
+        <v>32916</v>
+      </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="1">
+        <v>32860</v>
+      </c>
+      <c r="E12" s="17">
+        <v>56</v>
+      </c>
       <c r="F12" s="1"/>
+      <c r="I12">
+        <v>1.55</v>
+      </c>
+      <c r="N12">
+        <v>2.27712819427546</v>
+      </c>
+      <c r="R12">
+        <v>196.31271714018646</v>
+      </c>
     </row>
     <row r="13" spans="1:94" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1">
+        <v>32937</v>
+      </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="1">
+        <v>32860</v>
+      </c>
+      <c r="E13" s="17">
+        <v>77</v>
+      </c>
       <c r="F13" s="1"/>
+      <c r="I13">
+        <v>1.64</v>
+      </c>
+      <c r="N13">
+        <v>44.673474066627797</v>
+      </c>
+      <c r="R13">
+        <v>292.38382448900381</v>
+      </c>
     </row>
     <row r="14" spans="1:94" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1">
+        <v>32972</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1">
+        <v>32860</v>
+      </c>
+      <c r="E14" s="17">
+        <v>112</v>
+      </c>
       <c r="F14" s="1"/>
+      <c r="I14">
+        <v>1.3</v>
+      </c>
+      <c r="N14">
+        <v>69.633000017635794</v>
+      </c>
+      <c r="R14">
+        <v>298.91892845175676</v>
+      </c>
     </row>
     <row r="15" spans="1:94" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2"/>
@@ -3173,4 +3326,244 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF85533-17D7-4D6F-8FB1-C0833BDF5434}">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1">
+        <f>DATE(1989,12,18)+35</f>
+        <v>32895</v>
+      </c>
+      <c r="B2">
+        <v>35.121951219512098</v>
+      </c>
+      <c r="C2">
+        <v>-1.0708428125495799</v>
+      </c>
+      <c r="D2">
+        <v>34.878048780487802</v>
+      </c>
+      <c r="E2">
+        <v>69.212563709151098</v>
+      </c>
+      <c r="F2">
+        <f>E2+C2</f>
+        <v>68.141720896601512</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1">
+        <f>DATE(1989,12,18)+56</f>
+        <v>32916</v>
+      </c>
+      <c r="B3">
+        <v>56.341463414634099</v>
+      </c>
+      <c r="C3">
+        <v>2.27712819427546</v>
+      </c>
+      <c r="D3">
+        <v>56.097560975609703</v>
+      </c>
+      <c r="E3">
+        <v>194.035588945911</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="0">E3+C3</f>
+        <v>196.31271714018646</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
+        <f>DATE(1989,12,18)+77</f>
+        <v>32937</v>
+      </c>
+      <c r="B4">
+        <v>77.073170731707293</v>
+      </c>
+      <c r="C4">
+        <v>44.673474066627797</v>
+      </c>
+      <c r="D4">
+        <v>77.073170731707293</v>
+      </c>
+      <c r="E4">
+        <v>247.710350422376</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>292.38382448900381</v>
+      </c>
+      <c r="M4">
+        <v>1.2089697757555899</v>
+      </c>
+      <c r="N4">
+        <v>62.207604809879697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1">
+        <f>DATE(1989,12,18)+112</f>
+        <v>32972</v>
+      </c>
+      <c r="B5">
+        <v>112.19512195121899</v>
+      </c>
+      <c r="C5">
+        <v>69.633000017635794</v>
+      </c>
+      <c r="D5">
+        <v>112.19512195121899</v>
+      </c>
+      <c r="E5">
+        <v>229.28592843412099</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>298.91892845175676</v>
+      </c>
+      <c r="M5">
+        <v>23.140721481962899</v>
+      </c>
+      <c r="N5">
+        <v>58.288462788430202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M6">
+        <v>28.912577185570299</v>
+      </c>
+      <c r="N6">
+        <v>90.993045173870598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M7">
+        <v>34.596035099122503</v>
+      </c>
+      <c r="N7">
+        <v>70.331881702957403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M8">
+        <v>37.455313617159497</v>
+      </c>
+      <c r="N8">
+        <v>62.654793630159197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M9">
+        <v>41.112122196945002</v>
+      </c>
+      <c r="N9">
+        <v>55.564250893727603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M10">
+        <v>45.311667208319697</v>
+      </c>
+      <c r="N10">
+        <v>50.5354566135846</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M11">
+        <v>51.347416314592103</v>
+      </c>
+      <c r="N11">
+        <v>43.140721481962899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M12">
+        <v>58.410139746506303</v>
+      </c>
+      <c r="N12">
+        <v>31.024504387390301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M13">
+        <v>64.963275918101999</v>
+      </c>
+      <c r="N13">
+        <v>21.858693532661601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M14">
+        <v>72.074748131296701</v>
+      </c>
+      <c r="N14">
+        <v>17.1132921676958</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M15">
+        <v>80.005199870003196</v>
+      </c>
+      <c r="N15">
+        <v>16.197595060123501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M16">
+        <v>86.042898927526707</v>
+      </c>
+      <c r="N16">
+        <v>9.0976925576860594</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M17">
+        <v>96.830679233019097</v>
+      </c>
+      <c r="N17">
+        <v>0.21007474813129001</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="M18">
+        <v>106.877478063048</v>
+      </c>
+      <c r="N18">
+        <v>-0.71394215144621798</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Loxton,Roseworthy and Kingaroy8384 updated
</commit_message>
<xml_diff>
--- a/Prototypes/Peanut/Observed.xlsx
+++ b/Prototypes/Peanut/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Peanut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C1CD31-0ABA-462A-918A-C9751DFED51A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27CB0AB-5CFE-439E-855D-416826825585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="142">
   <si>
     <t>SimulationName</t>
   </si>
@@ -372,6 +372,105 @@
   <si>
     <t>Branch*</t>
   </si>
+  <si>
+    <t>Kingaroy8384SowSep28CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowOct12CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowOct26CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowNov09CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowNov25CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowDec07CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowDec21CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowJan04CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowJan18CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowFeb01CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowFeb15CvVirginiaBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowOct12CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowOct26CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowNov09CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowNov25CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowDec07CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowDec21CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowJan04CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowJan18CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowFeb01CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowFeb15CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowSep28CvEarlyBunch</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowSep28CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowOct12CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowOct26CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowNov09CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowNov25CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowDec07CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowDec21CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowJan04CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowJan18CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowFeb01CvFlorunner</t>
+  </si>
+  <si>
+    <t>Kingaroy8384SowFeb15CvFlorunner</t>
+  </si>
 </sst>
 </file>
 
@@ -434,7 +533,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -470,6 +569,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3472,10 +3573,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ394"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="A232" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="10236" activePane="topRight"/>
+      <selection activeCell="A254" sqref="A244:A254"/>
+      <selection pane="topRight" activeCell="E244" sqref="E244:E254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3922,6 +4023,10 @@
       <c r="Y11" s="1">
         <v>31.930050346738302</v>
       </c>
+      <c r="Z11" s="1">
+        <f>S11/X11</f>
+        <v>0.45825656659652136</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -4075,7 +4180,7 @@
         <v>29.815629620329101</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>29</v>
       </c>
@@ -4107,8 +4212,12 @@
       <c r="Y17" s="1">
         <v>32.7096544048214</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z17" s="1">
+        <f>S17/X17</f>
+        <v>0.56647955764075453</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>30</v>
       </c>
@@ -4136,7 +4245,7 @@
         <v>1.64304914565812</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
@@ -4170,7 +4279,7 @@
         <v>4.9005618213657103</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
@@ -4201,7 +4310,7 @@
         <v>9.1869781064637497</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
@@ -4232,7 +4341,7 @@
         <v>21.709765874464299</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>30</v>
       </c>
@@ -4264,8 +4373,12 @@
       <c r="Y22" s="1">
         <v>29.5099835207143</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z22" s="1">
+        <f>S22/X22</f>
+        <v>0.44095808953351817</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>30</v>
       </c>
@@ -4283,7 +4396,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>31</v>
       </c>
@@ -4305,7 +4418,7 @@
         <v>3.3757226576011199</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
@@ -4330,7 +4443,7 @@
         <v>6.57918247708729</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
@@ -4355,7 +4468,7 @@
         <v>9.3131376048393797</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
@@ -4380,7 +4493,7 @@
         <v>22.994465909246099</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>31</v>
       </c>
@@ -4407,7 +4520,7 @@
         <v>25.333346900617901</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
@@ -4428,7 +4541,7 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>32</v>
       </c>
@@ -4460,7 +4573,7 @@
         <v>2.9336266960030999</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>32</v>
       </c>
@@ -4492,7 +4605,7 @@
         <v>27.781444811147999</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>32</v>
       </c>
@@ -4527,7 +4640,7 @@
         <v>171.523285661899</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
@@ -4562,7 +4675,7 @@
         <v>458.39090575724202</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
@@ -4597,7 +4710,7 @@
         <v>640.95636230289699</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>32</v>
       </c>
@@ -4636,8 +4749,12 @@
       <c r="X35" s="1">
         <v>850.89842317565103</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z35" s="1">
+        <f>S35/X35</f>
+        <v>0.56175917945181852</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
@@ -4669,7 +4786,7 @@
         <v>12.5735240190683</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>33</v>
       </c>
@@ -4701,7 +4818,7 @@
         <v>49.748441510817599</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>33</v>
       </c>
@@ -4736,7 +4853,7 @@
         <v>234.68426842684201</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>33</v>
       </c>
@@ -4772,7 +4889,7 @@
         <v>509.43601026769301</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>33</v>
       </c>
@@ -4807,7 +4924,7 @@
         <v>660.44737807113995</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>33</v>
       </c>
@@ -4846,8 +4963,12 @@
       <c r="X41" s="1">
         <v>606.05207187385395</v>
       </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z41" s="1">
+        <f>S41/X41</f>
+        <v>0.44715629659031508</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>34</v>
       </c>
@@ -4879,7 +5000,7 @@
         <v>15.1023102310232</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>34</v>
       </c>
@@ -4911,7 +5032,7 @@
         <v>69.133846718005003</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>34</v>
       </c>
@@ -4946,7 +5067,7 @@
         <v>224.93876054272101</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>34</v>
       </c>
@@ -4981,7 +5102,7 @@
         <v>487.52181884855099</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>34</v>
       </c>
@@ -5016,7 +5137,7 @@
         <v>539.18298496516297</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>34</v>
       </c>
@@ -5055,8 +5176,12 @@
       <c r="X47" s="1">
         <v>720.04693802713598</v>
       </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z47" s="1">
+        <f>S47/X47</f>
+        <v>0.34442199098783444</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>35</v>
       </c>
@@ -5088,7 +5213,7 @@
         <v>17.367070040337399</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>35</v>
       </c>
@@ -5120,7 +5245,7 @@
         <v>102.952695269526</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>35</v>
       </c>
@@ -5155,7 +5280,7 @@
         <v>285.518151815181</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>35</v>
       </c>
@@ -5190,7 +5315,7 @@
         <v>574.650531719838</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>35</v>
       </c>
@@ -5225,7 +5350,7 @@
         <v>589.964063072974</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>35</v>
       </c>
@@ -5264,8 +5389,12 @@
       <c r="X53" s="1">
         <v>872.39017235056804</v>
       </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z53" s="1">
+        <f>S53/X53</f>
+        <v>0.43673119216076633</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>36</v>
       </c>
@@ -5297,7 +5426,7 @@
         <v>27.1653832049873</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>36</v>
       </c>
@@ -5329,7 +5458,7 @@
         <v>119.91492482581501</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>36</v>
       </c>
@@ -5364,7 +5493,7 @@
         <v>404.14814814814798</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>36</v>
       </c>
@@ -5399,7 +5528,7 @@
         <v>613.47414741474097</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>36</v>
       </c>
@@ -5435,7 +5564,7 @@
         <v>672.457645764576</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>36</v>
       </c>
@@ -5474,8 +5603,12 @@
       <c r="X59" s="1">
         <v>896.99156582324895</v>
       </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z59" s="1">
+        <f>S59/X59</f>
+        <v>0.34225516905305436</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>37</v>
       </c>
@@ -5507,7 +5640,7 @@
         <v>44.180418041804103</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>37</v>
       </c>
@@ -5539,7 +5672,7 @@
         <v>156.42097543087601</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>37</v>
       </c>
@@ -5574,7 +5707,7 @@
         <v>406.94096076274201</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>37</v>
       </c>
@@ -5609,7 +5742,7 @@
         <v>698.39090575724197</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>37</v>
       </c>
@@ -5644,7 +5777,7 @@
         <v>614.30143014301404</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>37</v>
       </c>
@@ -5683,8 +5816,12 @@
       <c r="X65" s="1">
         <v>925.964063072974</v>
       </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z65" s="1">
+        <f>S65/X65</f>
+        <v>0.34882563252840276</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
         <v>38</v>
       </c>
@@ -5713,7 +5850,7 @@
         <v>14.1576376953573</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
         <v>38</v>
       </c>
@@ -5742,7 +5879,7 @@
         <v>38.1365759029174</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>38</v>
       </c>
@@ -5771,7 +5908,7 @@
         <v>103.251645148664</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
         <v>38</v>
       </c>
@@ -5800,7 +5937,7 @@
         <v>269.36486443780501</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>38</v>
       </c>
@@ -5829,7 +5966,7 @@
         <v>402.49829225424799</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>38</v>
       </c>
@@ -5858,7 +5995,7 @@
         <v>471.77029421845998</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>38</v>
       </c>
@@ -5901,8 +6038,12 @@
       <c r="X72" s="1">
         <v>722.25393267713696</v>
       </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z72" s="1">
+        <f>S72/X72</f>
+        <v>0.55755403529442404</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
         <v>39</v>
       </c>
@@ -5931,7 +6072,7 @@
         <v>14.197019163216501</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
         <v>39</v>
       </c>
@@ -5960,7 +6101,7 @@
         <v>38.175957370776501</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
         <v>39</v>
       </c>
@@ -5989,7 +6130,7 @@
         <v>86.781440146246197</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
         <v>39</v>
       </c>
@@ -6018,7 +6159,7 @@
         <v>195.24894192692</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
         <v>39</v>
       </c>
@@ -6047,7 +6188,7 @@
         <v>332.49992099396798</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
         <v>39</v>
       </c>
@@ -6076,7 +6217,7 @@
         <v>430.59478171241301</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
         <v>39</v>
       </c>
@@ -6119,8 +6260,12 @@
       <c r="X79" s="1">
         <v>573.90394325179</v>
       </c>
-    </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z79" s="1">
+        <f>S79/X79</f>
+        <v>0.57364638814782731</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
         <v>40</v>
       </c>
@@ -6149,7 +6294,7 @@
         <v>16.216413320659701</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
         <v>40</v>
       </c>
@@ -6178,7 +6323,7 @@
         <v>31.960249027010299</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
         <v>40</v>
       </c>
@@ -6207,7 +6352,7 @@
         <v>78.506956177177699</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
         <v>40</v>
       </c>
@@ -6236,7 +6381,7 @@
         <v>141.72077566905901</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
         <v>40</v>
       </c>
@@ -6265,7 +6410,7 @@
         <v>241.874412012806</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
         <v>40</v>
       </c>
@@ -6294,7 +6439,7 @@
         <v>259.59826040873997</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
         <v>40</v>
       </c>
@@ -6330,8 +6475,12 @@
       <c r="X86" s="1">
         <v>405.08434197699802</v>
       </c>
-    </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z86" s="1">
+        <f>S86/X86</f>
+        <v>0.60964305392848284</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
         <v>41</v>
       </c>
@@ -6360,7 +6509,7 @@
         <v>16.216413320659701</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
         <v>41</v>
       </c>
@@ -6389,7 +6538,7 @@
         <v>27.842697776405601</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
         <v>41</v>
       </c>
@@ -6418,7 +6567,7 @@
         <v>57.9191999241541</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
         <v>41</v>
       </c>
@@ -6447,7 +6596,7 @@
         <v>125.211189198781</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
         <v>41</v>
       </c>
@@ -6476,7 +6625,7 @@
         <v>198.48259801002001</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
         <v>41</v>
       </c>
@@ -6505,7 +6654,7 @@
         <v>257.46072184771901</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
         <v>41</v>
       </c>
@@ -6541,8 +6690,12 @@
       <c r="X93" s="1">
         <v>343.28169175006798</v>
       </c>
-    </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z93" s="1">
+        <f t="shared" ref="Z93:Z101" si="8">S93/X93</f>
+        <v>0.61517153956727488</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
         <v>42</v>
       </c>
@@ -6578,8 +6731,12 @@
       <c r="X94" s="1">
         <v>1047.5702821131399</v>
       </c>
-    </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z94" s="1">
+        <f t="shared" si="8"/>
+        <v>0.5877198616698468</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
         <v>43</v>
       </c>
@@ -6615,8 +6772,12 @@
       <c r="X95" s="1">
         <v>796.46496972084105</v>
       </c>
-    </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z95" s="1">
+        <f t="shared" si="8"/>
+        <v>0.59785332049875728</v>
+      </c>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
         <v>44</v>
       </c>
@@ -6652,8 +6813,12 @@
       <c r="X96" s="1">
         <v>699.06221414893105</v>
       </c>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z96" s="1">
+        <f t="shared" si="8"/>
+        <v>0.5966570064180915</v>
+      </c>
+    </row>
+    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
         <v>45</v>
       </c>
@@ -6689,8 +6854,12 @@
       <c r="X97" s="1">
         <v>655.12957718011205</v>
       </c>
-    </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z97" s="1">
+        <f t="shared" si="8"/>
+        <v>0.58478450560410777</v>
+      </c>
+    </row>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
         <v>46</v>
       </c>
@@ -6726,8 +6895,12 @@
       <c r="X98" s="1">
         <v>1030.5631638546899</v>
       </c>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z98" s="1">
+        <f t="shared" si="8"/>
+        <v>0.57435408989559844</v>
+      </c>
+    </row>
+    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="s">
         <v>47</v>
       </c>
@@ -6763,8 +6936,12 @@
       <c r="X99" s="1">
         <v>845.29513434514297</v>
       </c>
-    </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z99" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55432121382614619</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
         <v>48</v>
       </c>
@@ -6800,8 +6977,12 @@
       <c r="X100" s="1">
         <v>785.61059731698401</v>
       </c>
-    </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z100" s="1">
+        <f t="shared" si="8"/>
+        <v>0.56902564173601522</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
         <v>49</v>
       </c>
@@ -6837,14 +7018,18 @@
       <c r="X101" s="1">
         <v>716.45025122502898</v>
       </c>
-    </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z101" s="1">
+        <f t="shared" si="8"/>
+        <v>0.5415984268554952</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B102" s="9"/>
       <c r="C102" s="6">
-        <f t="shared" ref="C102:C107" si="8">E102+F102</f>
+        <f t="shared" ref="C102:C107" si="9">E102+F102</f>
         <v>35776</v>
       </c>
       <c r="D102" s="6"/>
@@ -6852,7 +7037,7 @@
         <v>35741</v>
       </c>
       <c r="F102" s="7">
-        <f t="shared" ref="F102:F107" si="9">H102+G102</f>
+        <f t="shared" ref="F102:F107" si="10">H102+G102</f>
         <v>35</v>
       </c>
       <c r="G102" s="2">
@@ -6870,13 +7055,13 @@
         <v>90.397904842567598</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B103" s="9"/>
       <c r="C103" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>35797</v>
       </c>
       <c r="D103" s="6"/>
@@ -6884,7 +7069,7 @@
         <v>35741</v>
       </c>
       <c r="F103" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>56</v>
       </c>
       <c r="G103" s="2">
@@ -6902,13 +7087,13 @@
         <v>201.456863083733</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A104" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B104" s="9"/>
       <c r="C104" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>35818</v>
       </c>
       <c r="D104" s="6"/>
@@ -6916,7 +7101,7 @@
         <v>35741</v>
       </c>
       <c r="F104" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>77</v>
       </c>
       <c r="G104" s="2">
@@ -6934,13 +7119,13 @@
         <v>352.78798360023501</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A105" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B105" s="9"/>
       <c r="C105" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>35839</v>
       </c>
       <c r="D105" s="6"/>
@@ -6948,7 +7133,7 @@
         <v>35741</v>
       </c>
       <c r="F105" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>98</v>
       </c>
       <c r="G105" s="2">
@@ -6966,13 +7151,13 @@
         <v>661.62071877905498</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A106" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B106" s="9"/>
       <c r="C106" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>35860</v>
       </c>
       <c r="D106" s="6"/>
@@ -6980,7 +7165,7 @@
         <v>35741</v>
       </c>
       <c r="F106" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>119</v>
       </c>
       <c r="G106" s="2">
@@ -6998,13 +7183,13 @@
         <v>967.39635997151504</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A107" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B107" s="9"/>
       <c r="C107" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>35881</v>
       </c>
       <c r="D107" s="6"/>
@@ -7012,7 +7197,7 @@
         <v>35741</v>
       </c>
       <c r="F107" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>140</v>
       </c>
       <c r="G107" s="2">
@@ -7029,8 +7214,12 @@
       <c r="X107" s="1">
         <v>1124.9410322956101</v>
       </c>
-    </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z107" s="1">
+        <f t="shared" ref="Z107:Z115" si="11">S107/X107</f>
+        <v>0.5164687627891642</v>
+      </c>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A108" s="9" t="s">
         <v>50</v>
       </c>
@@ -7066,8 +7255,12 @@
       <c r="X108" s="1">
         <v>1297.83741710808</v>
       </c>
-    </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z108" s="1">
+        <f t="shared" si="11"/>
+        <v>0.54760057573932719</v>
+      </c>
+    </row>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A109" s="9" t="s">
         <v>51</v>
       </c>
@@ -7103,8 +7296,12 @@
       <c r="X109" s="1">
         <v>1135.43192825251</v>
       </c>
-    </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z109" s="1">
+        <f t="shared" si="11"/>
+        <v>0.55106873051835448</v>
+      </c>
+    </row>
+    <row r="110" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A110" s="9" t="s">
         <v>52</v>
       </c>
@@ -7140,8 +7337,12 @@
       <c r="X110" s="1">
         <v>1009.9101083416</v>
       </c>
-    </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z110" s="1">
+        <f t="shared" si="11"/>
+        <v>0.54152216496102545</v>
+      </c>
+    </row>
+    <row r="111" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A111" s="9" t="s">
         <v>53</v>
       </c>
@@ -7177,8 +7378,12 @@
       <c r="X111" s="1">
         <v>859.16057930755699</v>
       </c>
-    </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z111" s="1">
+        <f t="shared" si="11"/>
+        <v>0.52004526213321234</v>
+      </c>
+    </row>
+    <row r="112" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>54</v>
       </c>
@@ -7202,8 +7407,12 @@
       <c r="X112" s="1">
         <v>1261</v>
       </c>
-    </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z112" s="1">
+        <f t="shared" si="11"/>
+        <v>0.52101506740682002</v>
+      </c>
+    </row>
+    <row r="113" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>55</v>
       </c>
@@ -7227,8 +7436,12 @@
       <c r="X113" s="1">
         <v>1539</v>
       </c>
-    </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z113" s="1">
+        <f t="shared" si="11"/>
+        <v>0.41585445094217022</v>
+      </c>
+    </row>
+    <row r="114" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>56</v>
       </c>
@@ -7252,8 +7465,12 @@
       <c r="X114" s="1">
         <v>1556</v>
       </c>
-    </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z114" s="1">
+        <f t="shared" si="11"/>
+        <v>0.41902313624678661</v>
+      </c>
+    </row>
+    <row r="115" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>57</v>
       </c>
@@ -7277,8 +7494,12 @@
       <c r="X115" s="1">
         <v>1619</v>
       </c>
-    </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z115" s="1">
+        <f t="shared" si="11"/>
+        <v>0.35083384805435452</v>
+      </c>
+    </row>
+    <row r="116" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>54</v>
       </c>
@@ -7291,7 +7512,7 @@
         <v>3.3238030118388898E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>54</v>
       </c>
@@ -7304,7 +7525,7 @@
         <v>0.109379049467607</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>54</v>
       </c>
@@ -7317,7 +7538,7 @@
         <v>0.290782791382457</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>54</v>
       </c>
@@ -7330,7 +7551,7 @@
         <v>0.49097468445169801</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>54</v>
       </c>
@@ -7343,7 +7564,7 @@
         <v>0.82121824528124998</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>54</v>
       </c>
@@ -7356,7 +7577,7 @@
         <v>0.94371825906667095</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>54</v>
       </c>
@@ -7369,7 +7590,7 @@
         <v>0.980960954171744</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>55</v>
       </c>
@@ -7382,7 +7603,7 @@
         <v>9.7134837966153798E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>55</v>
       </c>
@@ -7395,7 +7616,7 @@
         <v>0.38504888310513802</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>55</v>
       </c>
@@ -7408,7 +7629,7 @@
         <v>0.66669193993967402</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>55</v>
       </c>
@@ -7421,7 +7642,7 @@
         <v>0.82806270712595997</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>55</v>
       </c>
@@ -7434,7 +7655,7 @@
         <v>0.94903116056707604</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>55</v>
       </c>
@@ -7662,7 +7883,7 @@
         <v>0.33</v>
       </c>
       <c r="M144" s="1">
-        <f t="shared" ref="M144:M173" si="10">L144/Q144</f>
+        <f t="shared" ref="M144:M173" si="12">L144/Q144</f>
         <v>2.4699999999999958E-2</v>
       </c>
       <c r="Q144" s="1">
@@ -7698,7 +7919,7 @@
         <v>1.06</v>
       </c>
       <c r="M145" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.12E-2</v>
       </c>
       <c r="Q145" s="1">
@@ -7735,7 +7956,7 @@
         <v>3.64</v>
       </c>
       <c r="M146" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.6999999999999962E-2</v>
       </c>
       <c r="Q146" s="1">
@@ -7771,7 +7992,7 @@
         <v>5.7</v>
       </c>
       <c r="M147" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.6399999999999989E-2</v>
       </c>
       <c r="Q147" s="1">
@@ -7807,7 +8028,7 @@
         <v>7.03</v>
       </c>
       <c r="M148" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.5400000000000006E-2</v>
       </c>
       <c r="Q148" s="1">
@@ -7853,7 +8074,7 @@
         <v>5.85</v>
       </c>
       <c r="M149" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.1499999999999995E-2</v>
       </c>
       <c r="Q149" s="1">
@@ -7867,6 +8088,10 @@
       </c>
       <c r="X149" s="1">
         <v>945.7</v>
+      </c>
+      <c r="Z149" s="1">
+        <f>S149/X149</f>
+        <v>0.37601776461880088</v>
       </c>
     </row>
     <row r="150" spans="1:26" x14ac:dyDescent="0.3">
@@ -7889,7 +8114,7 @@
         <v>0.71</v>
       </c>
       <c r="M150" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.0699999999999988E-2</v>
       </c>
       <c r="Q150" s="1">
@@ -7927,7 +8152,7 @@
         <v>1.43</v>
       </c>
       <c r="M151" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.8299999999999968E-2</v>
       </c>
       <c r="Q151" s="1">
@@ -7965,7 +8190,7 @@
         <v>4.53</v>
       </c>
       <c r="M152" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.9300000000000041E-2</v>
       </c>
       <c r="Q152" s="1">
@@ -8004,7 +8229,7 @@
         <v>7.77</v>
       </c>
       <c r="M153" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.6899999999999966E-2</v>
       </c>
       <c r="Q153" s="1">
@@ -8043,7 +8268,7 @@
         <v>6.14</v>
       </c>
       <c r="M154" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.2700000000000026E-2</v>
       </c>
       <c r="Q154" s="1">
@@ -8091,7 +8316,7 @@
         <v>3.12</v>
       </c>
       <c r="M155" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.1399999999999926E-2</v>
       </c>
       <c r="Q155" s="1">
@@ -8107,7 +8332,10 @@
         <v>1011.4</v>
       </c>
       <c r="Y155" s="12"/>
-      <c r="Z155" s="12"/>
+      <c r="Z155" s="1">
+        <f>S155/X155</f>
+        <v>0.45600158196559226</v>
+      </c>
     </row>
     <row r="156" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
@@ -8129,7 +8357,7 @@
         <v>0.49</v>
       </c>
       <c r="M156" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.7699999999999961E-2</v>
       </c>
       <c r="Q156" s="1">
@@ -8165,7 +8393,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="M157" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.6499999999999985E-2</v>
       </c>
       <c r="Q157" s="1">
@@ -8201,7 +8429,7 @@
         <v>2.93</v>
       </c>
       <c r="M158" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.3099999999999971E-2</v>
       </c>
       <c r="Q158" s="1">
@@ -8238,7 +8466,7 @@
         <v>4.28</v>
       </c>
       <c r="M159" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.9900000000000011E-2</v>
       </c>
       <c r="Q159" s="1">
@@ -8276,7 +8504,7 @@
         <v>4.7699999999999996</v>
       </c>
       <c r="M160" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.9300000000000036E-2</v>
       </c>
       <c r="Q160" s="1">
@@ -8292,7 +8520,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>62</v>
       </c>
@@ -8320,7 +8548,7 @@
         <v>4.3099999999999996</v>
       </c>
       <c r="M161" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.7200000000000014E-2</v>
       </c>
       <c r="Q161" s="1">
@@ -8335,8 +8563,12 @@
       <c r="X161" s="1">
         <v>1139.2</v>
       </c>
-    </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z161" s="1">
+        <f>S161/X161</f>
+        <v>0.4949964887640449</v>
+      </c>
+    </row>
+    <row r="162" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>64</v>
       </c>
@@ -8357,7 +8589,7 @@
         <v>0.36</v>
       </c>
       <c r="M162" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.0900000000000007E-2</v>
       </c>
       <c r="Q162" s="1">
@@ -8373,7 +8605,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>64</v>
       </c>
@@ -8394,7 +8626,7 @@
         <v>1.19</v>
       </c>
       <c r="M163" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.5599999999999998E-2</v>
       </c>
       <c r="Q163" s="1">
@@ -8410,7 +8642,7 @@
         <v>87.3</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>64</v>
       </c>
@@ -8431,7 +8663,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="M164" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.9499999999999979E-2</v>
       </c>
       <c r="Q164" s="1">
@@ -8447,7 +8679,7 @@
         <v>260.89999999999998</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>64</v>
       </c>
@@ -8468,7 +8700,7 @@
         <v>2.98</v>
       </c>
       <c r="M165" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.6800000000000034E-2</v>
       </c>
       <c r="Q165" s="1">
@@ -8484,7 +8716,7 @@
         <v>518.29999999999995</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>64</v>
       </c>
@@ -8504,7 +8736,7 @@
         <v>3.38</v>
       </c>
       <c r="M166" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.6399999999999981E-2</v>
       </c>
       <c r="Q166" s="1">
@@ -8520,7 +8752,7 @@
         <v>903.2</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>64</v>
       </c>
@@ -8551,7 +8783,7 @@
         <v>2.73</v>
       </c>
       <c r="M167" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.6699999999999954E-2</v>
       </c>
       <c r="Q167" s="1">
@@ -8566,8 +8798,12 @@
       <c r="X167" s="1">
         <v>810.1</v>
       </c>
-    </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z167" s="1">
+        <f>S167/X167</f>
+        <v>0.48500185162325632</v>
+      </c>
+    </row>
+    <row r="168" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>66</v>
       </c>
@@ -8587,7 +8823,7 @@
         <v>0.18</v>
       </c>
       <c r="M168" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.3200000000000005E-2</v>
       </c>
       <c r="Q168" s="1">
@@ -8603,7 +8839,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>66</v>
       </c>
@@ -8623,7 +8859,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M169" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.2100000000000002E-2</v>
       </c>
       <c r="Q169" s="1">
@@ -8639,7 +8875,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>66</v>
       </c>
@@ -8659,7 +8895,7 @@
         <v>1.91</v>
       </c>
       <c r="M170" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.8199999999999987E-2</v>
       </c>
       <c r="Q170" s="1">
@@ -8675,7 +8911,7 @@
         <v>235.4</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>66</v>
       </c>
@@ -8695,7 +8931,7 @@
         <v>2.44</v>
       </c>
       <c r="M171" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.6900000000000009E-2</v>
       </c>
       <c r="Q171" s="1">
@@ -8711,7 +8947,7 @@
         <v>438.2</v>
       </c>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>66</v>
       </c>
@@ -8732,7 +8968,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="M172" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.5200000000000021E-2</v>
       </c>
       <c r="Q172" s="1">
@@ -8748,7 +8984,7 @@
         <v>568.4</v>
       </c>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>66</v>
       </c>
@@ -8779,7 +9015,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="M173" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.7000000000000029E-2</v>
       </c>
       <c r="Q173" s="1">
@@ -8794,8 +9030,12 @@
       <c r="X173" s="1">
         <v>667.6</v>
       </c>
-    </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z173" s="1">
+        <f>S173/X173</f>
+        <v>0.57699221090473329</v>
+      </c>
+    </row>
+    <row r="174" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>68</v>
       </c>
@@ -8803,7 +9043,7 @@
         <v>69</v>
       </c>
       <c r="C174" s="6">
-        <f t="shared" ref="C174:C221" si="11">E174+F174</f>
+        <f t="shared" ref="C174:C221" si="13">E174+F174</f>
         <v>31023</v>
       </c>
       <c r="D174" s="6"/>
@@ -8827,7 +9067,7 @@
       </c>
       <c r="Y174" s="15"/>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>68</v>
       </c>
@@ -8835,7 +9075,7 @@
         <v>69</v>
       </c>
       <c r="C175" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31037</v>
       </c>
       <c r="E175" s="6">
@@ -8858,7 +9098,7 @@
       </c>
       <c r="Y175" s="16"/>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>68</v>
       </c>
@@ -8866,7 +9106,7 @@
         <v>69</v>
       </c>
       <c r="C176" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31051</v>
       </c>
       <c r="E176" s="6">
@@ -8889,7 +9129,7 @@
       </c>
       <c r="Y176" s="15"/>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>68</v>
       </c>
@@ -8897,7 +9137,7 @@
         <v>69</v>
       </c>
       <c r="C177" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31064</v>
       </c>
       <c r="E177" s="6">
@@ -8920,7 +9160,7 @@
       </c>
       <c r="Y177" s="15"/>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>68</v>
       </c>
@@ -8928,7 +9168,7 @@
         <v>69</v>
       </c>
       <c r="C178" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31078</v>
       </c>
       <c r="D178" s="13"/>
@@ -8949,7 +9189,7 @@
         <v>688.1</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>68</v>
       </c>
@@ -8957,7 +9197,7 @@
         <v>69</v>
       </c>
       <c r="C179" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31091</v>
       </c>
       <c r="D179" s="13"/>
@@ -8979,7 +9219,7 @@
         <v>866.2</v>
       </c>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>68</v>
       </c>
@@ -8987,7 +9227,7 @@
         <v>69</v>
       </c>
       <c r="C180" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31104</v>
       </c>
       <c r="D180" s="13"/>
@@ -9008,7 +9248,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>68</v>
       </c>
@@ -9016,7 +9256,7 @@
         <v>69</v>
       </c>
       <c r="C181" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31118</v>
       </c>
       <c r="D181" s="6" t="s">
@@ -9041,8 +9281,12 @@
       <c r="X181" s="1">
         <v>1055.4000000000001</v>
       </c>
-    </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z181" s="1">
+        <f>S181/X181</f>
+        <v>0.59001326511275343</v>
+      </c>
+    </row>
+    <row r="182" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>70</v>
       </c>
@@ -9050,7 +9294,7 @@
         <v>69</v>
       </c>
       <c r="C182" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31023</v>
       </c>
       <c r="D182" s="6"/>
@@ -9071,7 +9315,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>70</v>
       </c>
@@ -9079,7 +9323,7 @@
         <v>69</v>
       </c>
       <c r="C183" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31037</v>
       </c>
       <c r="E183" s="6">
@@ -9099,7 +9343,7 @@
         <v>177.7</v>
       </c>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>70</v>
       </c>
@@ -9107,7 +9351,7 @@
         <v>69</v>
       </c>
       <c r="C184" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31051</v>
       </c>
       <c r="E184" s="6">
@@ -9127,7 +9371,7 @@
         <v>387.5</v>
       </c>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>70</v>
       </c>
@@ -9135,7 +9379,7 @@
         <v>69</v>
       </c>
       <c r="C185" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31064</v>
       </c>
       <c r="E185" s="6">
@@ -9155,7 +9399,7 @@
         <v>616.20000000000005</v>
       </c>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>70</v>
       </c>
@@ -9163,7 +9407,7 @@
         <v>69</v>
       </c>
       <c r="C186" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31078</v>
       </c>
       <c r="D186" s="13"/>
@@ -9185,7 +9429,7 @@
         <v>806.9</v>
       </c>
     </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>70</v>
       </c>
@@ -9193,7 +9437,7 @@
         <v>69</v>
       </c>
       <c r="C187" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31091</v>
       </c>
       <c r="D187" s="13"/>
@@ -9214,7 +9458,7 @@
         <v>866.1</v>
       </c>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>70</v>
       </c>
@@ -9222,7 +9466,7 @@
         <v>69</v>
       </c>
       <c r="C188" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31104</v>
       </c>
       <c r="D188" s="13"/>
@@ -9243,7 +9487,7 @@
         <v>948.6</v>
       </c>
     </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>70</v>
       </c>
@@ -9251,7 +9495,7 @@
         <v>69</v>
       </c>
       <c r="C189" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31118</v>
       </c>
       <c r="D189" s="6" t="s">
@@ -9276,8 +9520,12 @@
       <c r="X189" s="1">
         <v>1032.8</v>
       </c>
-    </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z189" s="1">
+        <f>S189/X189</f>
+        <v>0.57000387296669253</v>
+      </c>
+    </row>
+    <row r="190" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>71</v>
       </c>
@@ -9285,7 +9533,7 @@
         <v>72</v>
       </c>
       <c r="C190" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31056</v>
       </c>
       <c r="D190" s="13"/>
@@ -9306,7 +9554,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
         <v>71</v>
       </c>
@@ -9314,7 +9562,7 @@
         <v>72</v>
       </c>
       <c r="C191" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31070</v>
       </c>
       <c r="D191" s="13"/>
@@ -9335,7 +9583,7 @@
         <v>178.8</v>
       </c>
     </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
         <v>71</v>
       </c>
@@ -9343,7 +9591,7 @@
         <v>72</v>
       </c>
       <c r="C192" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31084</v>
       </c>
       <c r="D192" s="13"/>
@@ -9364,7 +9612,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>71</v>
       </c>
@@ -9372,7 +9620,7 @@
         <v>72</v>
       </c>
       <c r="C193" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31104</v>
       </c>
       <c r="D193" s="13"/>
@@ -9394,7 +9642,7 @@
         <v>653.70000000000005</v>
       </c>
     </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
         <v>71</v>
       </c>
@@ -9402,7 +9650,7 @@
         <v>72</v>
       </c>
       <c r="C194" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31118</v>
       </c>
       <c r="D194" s="13"/>
@@ -9423,7 +9671,7 @@
         <v>894.2</v>
       </c>
     </row>
-    <row r="195" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
         <v>71</v>
       </c>
@@ -9431,7 +9679,7 @@
         <v>72</v>
       </c>
       <c r="C195" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31134</v>
       </c>
       <c r="D195" s="13"/>
@@ -9452,7 +9700,7 @@
         <v>1148.0999999999999</v>
       </c>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>71</v>
       </c>
@@ -9460,7 +9708,7 @@
         <v>72</v>
       </c>
       <c r="C196" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31148</v>
       </c>
       <c r="D196" s="13"/>
@@ -9481,7 +9729,7 @@
         <v>1135.8</v>
       </c>
     </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>71</v>
       </c>
@@ -9489,7 +9737,7 @@
         <v>72</v>
       </c>
       <c r="C197" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31161</v>
       </c>
       <c r="D197" s="6" t="s">
@@ -9514,8 +9762,12 @@
       <c r="X197" s="1">
         <v>1194.5999999999999</v>
       </c>
-    </row>
-    <row r="198" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z197" s="1">
+        <f>S197/X197</f>
+        <v>0.56002009040683076</v>
+      </c>
+    </row>
+    <row r="198" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>73</v>
       </c>
@@ -9523,7 +9775,7 @@
         <v>72</v>
       </c>
       <c r="C198" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31056</v>
       </c>
       <c r="D198" s="13"/>
@@ -9544,7 +9796,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="199" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>73</v>
       </c>
@@ -9552,7 +9804,7 @@
         <v>72</v>
       </c>
       <c r="C199" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31070</v>
       </c>
       <c r="D199" s="13"/>
@@ -9573,7 +9825,7 @@
         <v>239.5</v>
       </c>
     </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
         <v>73</v>
       </c>
@@ -9581,7 +9833,7 @@
         <v>72</v>
       </c>
       <c r="C200" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31084</v>
       </c>
       <c r="D200" s="13"/>
@@ -9603,7 +9855,7 @@
         <v>419.8</v>
       </c>
     </row>
-    <row r="201" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>73</v>
       </c>
@@ -9611,7 +9863,7 @@
         <v>72</v>
       </c>
       <c r="C201" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31104</v>
       </c>
       <c r="D201" s="13"/>
@@ -9632,7 +9884,7 @@
         <v>807.7</v>
       </c>
     </row>
-    <row r="202" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>73</v>
       </c>
@@ -9640,7 +9892,7 @@
         <v>72</v>
       </c>
       <c r="C202" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31118</v>
       </c>
       <c r="D202" s="13"/>
@@ -9661,7 +9913,7 @@
         <v>971.8</v>
       </c>
     </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
         <v>73</v>
       </c>
@@ -9669,7 +9921,7 @@
         <v>72</v>
       </c>
       <c r="C203" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31134</v>
       </c>
       <c r="D203" s="13"/>
@@ -9690,7 +9942,7 @@
         <v>1113.5999999999999</v>
       </c>
     </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>73</v>
       </c>
@@ -9698,7 +9950,7 @@
         <v>72</v>
       </c>
       <c r="C204" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31148</v>
       </c>
       <c r="D204" s="13"/>
@@ -9719,7 +9971,7 @@
         <v>1123.5999999999999</v>
       </c>
     </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
         <v>73</v>
       </c>
@@ -9727,7 +9979,7 @@
         <v>72</v>
       </c>
       <c r="C205" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31161</v>
       </c>
       <c r="D205" s="6" t="s">
@@ -9752,8 +10004,12 @@
       <c r="X205" s="1">
         <v>1290.3</v>
       </c>
-    </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z205" s="1">
+        <f>S205/X205</f>
+        <v>0.5600248004340076</v>
+      </c>
+    </row>
+    <row r="206" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>74</v>
       </c>
@@ -9761,7 +10017,7 @@
         <v>75</v>
       </c>
       <c r="C206" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31105</v>
       </c>
       <c r="D206" s="13"/>
@@ -9782,7 +10038,7 @@
         <v>83.7</v>
       </c>
     </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
         <v>74</v>
       </c>
@@ -9790,7 +10046,7 @@
         <v>75</v>
       </c>
       <c r="C207" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31113</v>
       </c>
       <c r="D207" s="13"/>
@@ -9812,7 +10068,7 @@
         <v>128.9</v>
       </c>
     </row>
-    <row r="208" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>74</v>
       </c>
@@ -9820,7 +10076,7 @@
         <v>75</v>
       </c>
       <c r="C208" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31127</v>
       </c>
       <c r="D208" s="13"/>
@@ -9849,7 +10105,7 @@
         <v>75</v>
       </c>
       <c r="C209" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31141</v>
       </c>
       <c r="D209" s="13"/>
@@ -9878,7 +10134,7 @@
         <v>75</v>
       </c>
       <c r="C210" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31162</v>
       </c>
       <c r="D210" s="13"/>
@@ -9907,7 +10163,7 @@
         <v>75</v>
       </c>
       <c r="C211" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31177</v>
       </c>
       <c r="D211" s="13"/>
@@ -9936,7 +10192,7 @@
         <v>75</v>
       </c>
       <c r="C212" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31189</v>
       </c>
       <c r="D212" s="13"/>
@@ -9965,7 +10221,7 @@
         <v>75</v>
       </c>
       <c r="C213" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31195</v>
       </c>
       <c r="D213" s="6" t="s">
@@ -9990,6 +10246,10 @@
       <c r="X213" s="1">
         <v>773.5</v>
       </c>
+      <c r="Z213" s="1">
+        <f>S213/X213</f>
+        <v>0.60995475113122177</v>
+      </c>
     </row>
     <row r="214" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
@@ -9999,7 +10259,7 @@
         <v>75</v>
       </c>
       <c r="C214" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31105</v>
       </c>
       <c r="D214" s="13"/>
@@ -10029,7 +10289,7 @@
         <v>75</v>
       </c>
       <c r="C215" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31113</v>
       </c>
       <c r="D215" s="13"/>
@@ -10058,7 +10318,7 @@
         <v>75</v>
       </c>
       <c r="C216" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31127</v>
       </c>
       <c r="D216" s="13"/>
@@ -10087,7 +10347,7 @@
         <v>75</v>
       </c>
       <c r="C217" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31141</v>
       </c>
       <c r="D217" s="13"/>
@@ -10116,7 +10376,7 @@
         <v>75</v>
       </c>
       <c r="C218" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31162</v>
       </c>
       <c r="D218" s="13"/>
@@ -10145,7 +10405,7 @@
         <v>75</v>
       </c>
       <c r="C219" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31177</v>
       </c>
       <c r="D219" s="13"/>
@@ -10174,7 +10434,7 @@
         <v>75</v>
       </c>
       <c r="C220" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31189</v>
       </c>
       <c r="D220" s="13"/>
@@ -10203,7 +10463,7 @@
         <v>75</v>
       </c>
       <c r="C221" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31195</v>
       </c>
       <c r="D221" s="6" t="s">
@@ -10229,200 +10489,536 @@
       <c r="X221" s="1">
         <v>746.4</v>
       </c>
+      <c r="Z221" s="1">
+        <f>S221/X221</f>
+        <v>0.59994640943194</v>
+      </c>
     </row>
     <row r="222" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A222" s="21" t="s">
+        <v>109</v>
+      </c>
       <c r="C222" s="8"/>
-      <c r="D222" s="8"/>
-      <c r="E222" s="8"/>
+      <c r="D222" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E222" s="8">
+        <v>30587</v>
+      </c>
+      <c r="I222" s="1">
+        <v>50</v>
+      </c>
       <c r="CU222" s="2"/>
     </row>
     <row r="223" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A223" s="21" t="s">
+        <v>110</v>
+      </c>
       <c r="C223" s="8"/>
-      <c r="D223" s="8"/>
-      <c r="E223" s="8"/>
+      <c r="D223" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E223" s="8">
+        <v>30601</v>
+      </c>
+      <c r="I223" s="1">
+        <v>51</v>
+      </c>
       <c r="CU223" s="2"/>
     </row>
     <row r="224" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A224" s="21" t="s">
+        <v>111</v>
+      </c>
       <c r="C224" s="8"/>
-      <c r="D224" s="8"/>
-      <c r="E224" s="8"/>
+      <c r="D224" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E224" s="8">
+        <v>30615</v>
+      </c>
+      <c r="I224" s="1">
+        <v>49</v>
+      </c>
       <c r="CU224" s="2"/>
     </row>
-    <row r="225" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A225" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="C225" s="8"/>
-      <c r="D225" s="8"/>
-      <c r="E225" s="8"/>
+      <c r="D225" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E225" s="8">
+        <v>30629</v>
+      </c>
+      <c r="I225" s="22">
+        <v>48</v>
+      </c>
       <c r="CU225" s="2"/>
     </row>
-    <row r="226" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A226" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="C226" s="8"/>
-      <c r="D226" s="8"/>
-      <c r="E226" s="8"/>
+      <c r="D226" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E226" s="8">
+        <v>30645</v>
+      </c>
+      <c r="I226" s="22">
+        <v>42</v>
+      </c>
       <c r="CU226" s="2"/>
     </row>
-    <row r="227" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A227" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="C227" s="8"/>
-      <c r="D227" s="8"/>
-      <c r="E227" s="8"/>
+      <c r="D227" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E227" s="8">
+        <v>30657</v>
+      </c>
+      <c r="I227" s="22">
+        <v>42</v>
+      </c>
       <c r="CU227" s="2"/>
     </row>
-    <row r="228" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A228" s="21" t="s">
+        <v>115</v>
+      </c>
       <c r="C228" s="8"/>
-      <c r="D228" s="8"/>
-      <c r="E228" s="8"/>
+      <c r="D228" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E228" s="8">
+        <v>30671</v>
+      </c>
+      <c r="I228" s="22">
+        <v>38</v>
+      </c>
       <c r="CU228" s="2"/>
     </row>
-    <row r="229" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A229" s="21" t="s">
+        <v>116</v>
+      </c>
       <c r="C229" s="8"/>
-      <c r="D229" s="8"/>
-      <c r="E229" s="8"/>
+      <c r="D229" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E229" s="8">
+        <v>30685</v>
+      </c>
+      <c r="I229" s="22">
+        <v>38</v>
+      </c>
       <c r="CU229" s="2"/>
     </row>
-    <row r="230" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A230" s="21" t="s">
+        <v>117</v>
+      </c>
       <c r="C230" s="8"/>
-      <c r="D230" s="8"/>
-      <c r="E230" s="8"/>
+      <c r="D230" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E230" s="8">
+        <v>30699</v>
+      </c>
+      <c r="I230" s="22">
+        <v>42</v>
+      </c>
       <c r="CU230" s="2"/>
     </row>
-    <row r="231" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A231" s="21" t="s">
+        <v>118</v>
+      </c>
       <c r="C231" s="8"/>
-      <c r="D231" s="8"/>
-      <c r="E231" s="8"/>
+      <c r="D231" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E231" s="8">
+        <v>30713</v>
+      </c>
+      <c r="I231" s="22">
+        <v>40</v>
+      </c>
       <c r="CU231" s="2"/>
     </row>
-    <row r="232" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A232" s="21" t="s">
+        <v>119</v>
+      </c>
       <c r="C232" s="8"/>
-      <c r="D232" s="8"/>
-      <c r="E232" s="8"/>
+      <c r="D232" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E232" s="8">
+        <v>30727</v>
+      </c>
+      <c r="I232" s="22">
+        <v>44</v>
+      </c>
       <c r="CU232" s="2"/>
     </row>
-    <row r="233" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A233" s="21" t="s">
+        <v>130</v>
+      </c>
       <c r="C233" s="8"/>
-      <c r="D233" s="8"/>
-      <c r="E233" s="8"/>
+      <c r="D233" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E233" s="8">
+        <v>30587</v>
+      </c>
+      <c r="I233" s="22">
+        <v>49</v>
+      </c>
       <c r="CU233" s="2"/>
     </row>
-    <row r="234" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A234" s="21" t="s">
+        <v>120</v>
+      </c>
       <c r="C234" s="8"/>
-      <c r="D234" s="8"/>
-      <c r="E234" s="8"/>
+      <c r="D234" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E234" s="8">
+        <v>30601</v>
+      </c>
+      <c r="I234" s="22">
+        <v>50</v>
+      </c>
       <c r="CU234" s="2"/>
     </row>
-    <row r="235" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A235" s="21" t="s">
+        <v>121</v>
+      </c>
       <c r="C235" s="8"/>
-      <c r="D235" s="8"/>
-      <c r="E235" s="8"/>
+      <c r="D235" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E235" s="8">
+        <v>30615</v>
+      </c>
+      <c r="I235" s="22">
+        <v>47</v>
+      </c>
       <c r="CU235" s="2"/>
     </row>
-    <row r="236" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A236" s="21" t="s">
+        <v>122</v>
+      </c>
       <c r="C236" s="8"/>
-      <c r="D236" s="8"/>
-      <c r="E236" s="8"/>
+      <c r="D236" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E236" s="8">
+        <v>30629</v>
+      </c>
+      <c r="I236" s="22">
+        <v>46</v>
+      </c>
       <c r="CU236" s="2"/>
     </row>
-    <row r="237" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A237" s="21" t="s">
+        <v>123</v>
+      </c>
       <c r="C237" s="8"/>
-      <c r="D237" s="8"/>
-      <c r="E237" s="8"/>
+      <c r="D237" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E237" s="8">
+        <v>30645</v>
+      </c>
+      <c r="I237" s="22">
+        <v>43</v>
+      </c>
       <c r="CU237" s="2"/>
     </row>
-    <row r="238" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A238" s="21" t="s">
+        <v>124</v>
+      </c>
       <c r="C238" s="8"/>
-      <c r="D238" s="8"/>
-      <c r="E238" s="8"/>
+      <c r="D238" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E238" s="8">
+        <v>30657</v>
+      </c>
+      <c r="I238" s="22">
+        <v>43</v>
+      </c>
       <c r="CU238" s="2"/>
     </row>
-    <row r="239" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A239" s="21" t="s">
+        <v>125</v>
+      </c>
       <c r="C239" s="8"/>
-      <c r="D239" s="8"/>
-      <c r="E239" s="8"/>
+      <c r="D239" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E239" s="8">
+        <v>30671</v>
+      </c>
+      <c r="I239" s="22">
+        <v>38</v>
+      </c>
       <c r="CU239" s="2"/>
     </row>
-    <row r="240" spans="3:99" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A240" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="C240" s="8"/>
-      <c r="D240" s="8"/>
-      <c r="E240" s="8"/>
+      <c r="D240" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E240" s="8">
+        <v>30685</v>
+      </c>
+      <c r="I240" s="22">
+        <v>38</v>
+      </c>
       <c r="CU240" s="2"/>
     </row>
     <row r="241" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A241" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="C241" s="8"/>
-      <c r="D241" s="8"/>
-      <c r="E241" s="8"/>
+      <c r="D241" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E241" s="8">
+        <v>30699</v>
+      </c>
+      <c r="I241" s="22">
+        <v>39</v>
+      </c>
       <c r="CU241" s="2"/>
     </row>
     <row r="242" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A242" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="C242" s="8"/>
-      <c r="D242" s="8"/>
-      <c r="E242" s="8"/>
+      <c r="D242" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E242" s="8">
+        <v>30713</v>
+      </c>
+      <c r="I242" s="22">
+        <v>38</v>
+      </c>
       <c r="CU242" s="2"/>
     </row>
     <row r="243" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A243" s="21" t="s">
+        <v>129</v>
+      </c>
       <c r="C243" s="8"/>
-      <c r="D243" s="8"/>
-      <c r="E243" s="8"/>
+      <c r="D243" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E243" s="8">
+        <v>30727</v>
+      </c>
+      <c r="I243" s="22">
+        <v>40</v>
+      </c>
       <c r="CU243" s="2"/>
     </row>
     <row r="244" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A244" s="21" t="s">
+        <v>131</v>
+      </c>
       <c r="C244" s="8"/>
-      <c r="D244" s="8"/>
-      <c r="E244" s="8"/>
+      <c r="D244" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E244" s="8">
+        <v>30587</v>
+      </c>
+      <c r="I244" s="1">
+        <v>49</v>
+      </c>
       <c r="CU244" s="2"/>
     </row>
     <row r="245" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A245" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="C245" s="8"/>
-      <c r="D245" s="8"/>
-      <c r="E245" s="8"/>
+      <c r="D245" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E245" s="8">
+        <v>30601</v>
+      </c>
+      <c r="I245" s="1">
+        <v>49</v>
+      </c>
       <c r="CU245" s="2"/>
     </row>
     <row r="246" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A246" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="C246" s="8"/>
-      <c r="D246" s="8"/>
-      <c r="E246" s="8"/>
+      <c r="D246" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E246" s="8">
+        <v>30615</v>
+      </c>
+      <c r="I246" s="1">
+        <v>43</v>
+      </c>
       <c r="CU246" s="2"/>
     </row>
     <row r="247" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A247" s="21" t="s">
+        <v>134</v>
+      </c>
       <c r="C247" s="8"/>
-      <c r="D247" s="8"/>
-      <c r="E247" s="8"/>
+      <c r="D247" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E247" s="8">
+        <v>30629</v>
+      </c>
+      <c r="I247" s="22">
+        <v>45</v>
+      </c>
       <c r="CU247" s="2"/>
     </row>
     <row r="248" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A248" s="21" t="s">
+        <v>135</v>
+      </c>
       <c r="C248" s="8"/>
-      <c r="D248" s="8"/>
-      <c r="E248" s="8"/>
+      <c r="D248" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E248" s="8">
+        <v>30645</v>
+      </c>
+      <c r="I248" s="22">
+        <v>42</v>
+      </c>
       <c r="CU248" s="2"/>
     </row>
     <row r="249" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A249" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="C249" s="8"/>
-      <c r="D249" s="8"/>
-      <c r="E249" s="8"/>
+      <c r="D249" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E249" s="8">
+        <v>30657</v>
+      </c>
+      <c r="I249" s="22">
+        <v>38</v>
+      </c>
       <c r="CU249" s="2"/>
     </row>
     <row r="250" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A250" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="C250" s="8"/>
-      <c r="D250" s="8"/>
-      <c r="E250" s="8"/>
+      <c r="D250" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E250" s="8">
+        <v>30671</v>
+      </c>
+      <c r="I250" s="22">
+        <v>35</v>
+      </c>
       <c r="CU250" s="2"/>
     </row>
     <row r="251" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A251" s="21" t="s">
+        <v>138</v>
+      </c>
       <c r="C251" s="8"/>
-      <c r="D251" s="8"/>
-      <c r="E251" s="8"/>
+      <c r="D251" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E251" s="8">
+        <v>30685</v>
+      </c>
+      <c r="I251" s="22">
+        <v>36</v>
+      </c>
       <c r="CU251" s="2"/>
     </row>
     <row r="252" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A252" s="21" t="s">
+        <v>139</v>
+      </c>
       <c r="C252" s="8"/>
-      <c r="D252" s="8"/>
-      <c r="E252" s="8"/>
+      <c r="D252" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E252" s="8">
+        <v>30699</v>
+      </c>
+      <c r="I252" s="22">
+        <v>38</v>
+      </c>
       <c r="CU252" s="2"/>
     </row>
     <row r="253" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="A253" s="5"/>
-      <c r="B253" s="5"/>
-      <c r="I253" s="8"/>
+      <c r="A253" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C253" s="8"/>
+      <c r="D253" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E253" s="8">
+        <v>30713</v>
+      </c>
+      <c r="I253" s="22">
+        <v>37</v>
+      </c>
     </row>
     <row r="254" spans="1:99" x14ac:dyDescent="0.3">
-      <c r="I254" s="8"/>
+      <c r="A254" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C254" s="8"/>
+      <c r="D254" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E254" s="8">
+        <v>30727</v>
+      </c>
+      <c r="I254" s="22">
+        <v>38</v>
+      </c>
     </row>
     <row r="255" spans="1:99" x14ac:dyDescent="0.3">
       <c r="I255" s="8"/>
@@ -13948,7 +14544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C3:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -14025,7 +14621,7 @@
         <v>2.6987098061752675</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F18" si="3">F6+1</f>
+        <f t="shared" ref="F7:F9" si="3">F6+1</f>
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Not sure if this is progress
added Headland met data and determined headland sowing date.  Trying to get model working at all locations
</commit_message>
<xml_diff>
--- a/Prototypes/Peanut/Observed.xlsx
+++ b/Prototypes/Peanut/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Peanut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8905039-24A5-43D5-9BA1-CF9151B50236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1483B5-8ECD-4F1A-8E35-23DC55A2CB06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3624,7 +3624,7 @@
       <pane xSplit="8" ySplit="2" topLeftCell="P263" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC270" sqref="AC270"/>
+      <selection pane="bottomRight" activeCell="C264" sqref="C264:C275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11248,8 +11248,8 @@
         <v>153</v>
       </c>
       <c r="C264" s="23">
-        <f>DATE(1988,9,28)+F264</f>
-        <v>32448</v>
+        <f>DATE(1988,4,28)+F264</f>
+        <v>32295</v>
       </c>
       <c r="F264" s="2">
         <v>34</v>
@@ -11297,8 +11297,8 @@
         <v>153</v>
       </c>
       <c r="C265" s="23">
-        <f t="shared" ref="C265:C275" si="14">DATE(1988,9,28)+F265</f>
-        <v>32455</v>
+        <f t="shared" ref="C265:C275" si="14">DATE(1988,4,28)+F265</f>
+        <v>32302</v>
       </c>
       <c r="F265" s="2">
         <f>F264+7</f>
@@ -11348,7 +11348,7 @@
       </c>
       <c r="C266" s="23">
         <f t="shared" si="14"/>
-        <v>32462</v>
+        <v>32309</v>
       </c>
       <c r="F266" s="2">
         <f t="shared" ref="F266:F275" si="18">F265+7</f>
@@ -11398,7 +11398,7 @@
       </c>
       <c r="C267" s="23">
         <f t="shared" si="14"/>
-        <v>32469</v>
+        <v>32316</v>
       </c>
       <c r="F267" s="2">
         <f t="shared" si="18"/>
@@ -11448,7 +11448,7 @@
       </c>
       <c r="C268" s="23">
         <f t="shared" si="14"/>
-        <v>32476</v>
+        <v>32323</v>
       </c>
       <c r="F268" s="2">
         <f t="shared" si="18"/>
@@ -11498,7 +11498,7 @@
       </c>
       <c r="C269" s="23">
         <f t="shared" si="14"/>
-        <v>32483</v>
+        <v>32330</v>
       </c>
       <c r="F269" s="2">
         <f t="shared" si="18"/>
@@ -11548,7 +11548,7 @@
       </c>
       <c r="C270" s="23">
         <f t="shared" si="14"/>
-        <v>32490</v>
+        <v>32337</v>
       </c>
       <c r="F270" s="2">
         <f t="shared" si="18"/>
@@ -11562,7 +11562,7 @@
       </c>
       <c r="C271" s="23">
         <f t="shared" si="14"/>
-        <v>32497</v>
+        <v>32344</v>
       </c>
       <c r="F271" s="2">
         <f t="shared" si="18"/>
@@ -11612,7 +11612,7 @@
       </c>
       <c r="C272" s="23">
         <f t="shared" si="14"/>
-        <v>32504</v>
+        <v>32351</v>
       </c>
       <c r="F272" s="2">
         <f t="shared" si="18"/>
@@ -11662,7 +11662,7 @@
       </c>
       <c r="C273" s="23">
         <f t="shared" si="14"/>
-        <v>32511</v>
+        <v>32358</v>
       </c>
       <c r="F273" s="2">
         <f t="shared" si="18"/>
@@ -11712,7 +11712,7 @@
       </c>
       <c r="C274" s="23">
         <f t="shared" si="14"/>
-        <v>32518</v>
+        <v>32365</v>
       </c>
       <c r="F274" s="2">
         <f t="shared" si="18"/>
@@ -11762,7 +11762,7 @@
       </c>
       <c r="C275" s="23">
         <f t="shared" si="14"/>
-        <v>32525</v>
+        <v>32372</v>
       </c>
       <c r="D275" s="6" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Fixed dates in datasets 8990 Qld
</commit_message>
<xml_diff>
--- a/Prototypes/Peanut/Observed.xlsx
+++ b/Prototypes/Peanut/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Peanut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50E049B-CCE8-4367-B845-8822C11DC300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2A1E5F-5741-4B24-B708-5E5E562126FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="12346" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3640,11 +3640,11 @@
   <dimension ref="A1:AMK392"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10927" ySplit="1147" topLeftCell="R327" activePane="bottomRight"/>
+      <pane xSplit="10927" ySplit="1147" topLeftCell="E317" activePane="bottomRight"/>
       <selection activeCell="D1" sqref="A1:XFD1"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="D327" sqref="D327"/>
-      <selection pane="bottomRight" activeCell="T340" sqref="T340"/>
+      <selection pane="bottomLeft" activeCell="A334" sqref="A334"/>
+      <selection pane="bottomRight" activeCell="H340" sqref="H340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3920,16 +3920,19 @@
       <c r="B6" s="5"/>
       <c r="C6" s="6">
         <f t="shared" ref="C6:C37" si="0">E6+F6</f>
-        <v>32882</v>
+        <v>32892</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6">
         <v>32854</v>
       </c>
       <c r="F6" s="7">
+        <f>G6+10</f>
+        <v>38</v>
+      </c>
+      <c r="G6" s="7">
         <v>28</v>
       </c>
-      <c r="G6" s="7"/>
       <c r="H6" s="6"/>
       <c r="T6" s="1">
         <v>0</v>
@@ -3948,16 +3951,19 @@
       <c r="B7" s="5"/>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>32896</v>
+        <v>32906</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6">
         <v>32854</v>
       </c>
       <c r="F7" s="7">
+        <f t="shared" ref="F7:F29" si="1">G7+10</f>
+        <v>52</v>
+      </c>
+      <c r="G7" s="7">
         <v>42</v>
       </c>
-      <c r="G7" s="7"/>
       <c r="H7" s="6"/>
       <c r="T7" s="1">
         <v>4.9439358603006403</v>
@@ -3979,16 +3985,19 @@
       <c r="B8" s="5"/>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>32909</v>
+        <v>32919</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6">
         <v>32854</v>
       </c>
       <c r="F8" s="7">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="G8" s="7">
         <v>55</v>
       </c>
-      <c r="G8" s="7"/>
       <c r="H8" s="6"/>
       <c r="T8" s="1">
         <v>29.7172309045791</v>
@@ -4010,16 +4019,19 @@
       <c r="B9" s="5"/>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>32929</v>
+        <v>32939</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6">
         <v>32854</v>
       </c>
       <c r="F9" s="7">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="G9" s="7">
         <v>75</v>
       </c>
-      <c r="G9" s="7"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -4045,16 +4057,19 @@
       <c r="B10" s="5"/>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>32944</v>
+        <v>32954</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6">
         <v>32854</v>
       </c>
       <c r="F10" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G10" s="7">
         <v>90</v>
       </c>
-      <c r="G10" s="7"/>
       <c r="H10" s="6"/>
       <c r="T10" s="1">
         <v>381.09646683874598</v>
@@ -4076,7 +4091,7 @@
       <c r="B11" s="5"/>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>32960</v>
+        <v>32970</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>26</v>
@@ -4085,10 +4100,15 @@
         <v>32854</v>
       </c>
       <c r="F11" s="7">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="G11" s="7">
         <v>106</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="7">
+        <v>10</v>
+      </c>
       <c r="T11" s="1">
         <v>518.33865894245798</v>
       </c>
@@ -4113,16 +4133,19 @@
       <c r="B12" s="5"/>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>32882</v>
+        <v>32892</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6">
         <v>32854</v>
       </c>
       <c r="F12" s="7">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="G12" s="7">
         <v>28</v>
       </c>
-      <c r="G12" s="7"/>
       <c r="H12" s="6"/>
       <c r="T12" s="1">
         <v>0</v>
@@ -4141,16 +4164,19 @@
       <c r="B13" s="5"/>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>32896</v>
+        <v>32906</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6">
         <v>32854</v>
       </c>
       <c r="F13" s="7">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="G13" s="7">
         <v>42</v>
       </c>
-      <c r="G13" s="7"/>
       <c r="H13" s="6"/>
       <c r="T13" s="1">
         <v>10.860009793588</v>
@@ -4172,16 +4198,19 @@
       <c r="B14" s="5"/>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>32909</v>
+        <v>32919</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6">
         <v>32854</v>
       </c>
       <c r="F14" s="7">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="G14" s="7">
         <v>55</v>
       </c>
-      <c r="G14" s="7"/>
       <c r="H14" s="6"/>
       <c r="T14" s="1">
         <v>63.314548457510199</v>
@@ -4203,16 +4232,19 @@
       <c r="B15" s="5"/>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>32929</v>
+        <v>32939</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
         <v>32854</v>
       </c>
       <c r="F15" s="7">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="G15" s="7">
         <v>75</v>
       </c>
-      <c r="G15" s="7"/>
       <c r="H15" s="6"/>
       <c r="T15" s="1">
         <v>356.457211151411</v>
@@ -4234,16 +4266,19 @@
       <c r="B16" s="5"/>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>32944</v>
+        <v>32954</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6">
         <v>32854</v>
       </c>
       <c r="F16" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G16" s="7">
         <v>90</v>
       </c>
-      <c r="G16" s="7"/>
       <c r="H16" s="6"/>
       <c r="T16" s="1">
         <v>570.86233369575098</v>
@@ -4265,7 +4300,7 @@
       <c r="B17" s="5"/>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>32960</v>
+        <v>32970</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>26</v>
@@ -4274,10 +4309,15 @@
         <v>32854</v>
       </c>
       <c r="F17" s="7">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="G17" s="7">
         <v>106</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="7">
+        <v>10</v>
+      </c>
       <c r="T17" s="1">
         <v>591.48464149659299</v>
       </c>
@@ -4302,16 +4342,19 @@
       <c r="B18" s="5"/>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>32882</v>
+        <v>32892</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6">
         <v>32854</v>
       </c>
       <c r="F18" s="7">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="G18" s="7">
         <v>28</v>
       </c>
-      <c r="G18" s="7"/>
       <c r="H18" s="6"/>
       <c r="T18" s="1">
         <v>0</v>
@@ -4330,16 +4373,19 @@
       <c r="B19" s="5"/>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>32896</v>
+        <v>32906</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6">
         <v>32854</v>
       </c>
       <c r="F19" s="7">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="G19" s="7">
         <v>42</v>
       </c>
-      <c r="G19" s="7"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -4365,16 +4411,19 @@
       <c r="B20" s="5"/>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>32909</v>
+        <v>32919</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6">
         <v>32854</v>
       </c>
       <c r="F20" s="7">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="G20" s="7">
         <v>55</v>
       </c>
-      <c r="G20" s="7"/>
       <c r="H20" s="6"/>
       <c r="T20" s="1">
         <v>71.235568982546098</v>
@@ -4396,16 +4445,19 @@
       <c r="B21" s="5"/>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>32929</v>
+        <v>32939</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6">
         <v>32854</v>
       </c>
       <c r="F21" s="7">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="G21" s="7">
         <v>75</v>
       </c>
-      <c r="G21" s="7"/>
       <c r="H21" s="6"/>
       <c r="T21" s="1">
         <v>307.02490725140501</v>
@@ -4427,19 +4479,18 @@
       <c r="B22" s="5"/>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>32944</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>26</v>
+        <v>32954</v>
       </c>
       <c r="E22" s="6">
         <v>32854</v>
       </c>
       <c r="F22" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G22" s="7">
         <v>90</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="6"/>
       <c r="T22" s="1">
         <v>444.358810494078</v>
       </c>
@@ -4464,16 +4515,24 @@
       <c r="B23" s="5"/>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>32960</v>
+        <v>32970</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="E23" s="6">
         <v>32854</v>
       </c>
       <c r="F23" s="7">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="G23" s="7">
         <v>106</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="7">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A24" s="5" t="s">
@@ -4482,16 +4541,19 @@
       <c r="B24" s="5"/>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>32882</v>
+        <v>32892</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6">
         <v>32854</v>
       </c>
       <c r="F24" s="7">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="G24" s="7">
         <v>28</v>
       </c>
-      <c r="G24" s="7"/>
       <c r="H24" s="6"/>
       <c r="Z24" s="1">
         <v>3.3757226576011199</v>
@@ -4504,16 +4566,19 @@
       <c r="B25" s="5"/>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>32896</v>
+        <v>32906</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6">
         <v>32854</v>
       </c>
       <c r="F25" s="7">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="G25" s="7">
         <v>42</v>
       </c>
-      <c r="G25" s="7"/>
       <c r="H25" s="6"/>
       <c r="U25" s="1">
         <v>0.62716694180183996</v>
@@ -4529,16 +4594,19 @@
       <c r="B26" s="5"/>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>32909</v>
+        <v>32919</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6">
         <v>32854</v>
       </c>
       <c r="F26" s="7">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="G26" s="7">
         <v>55</v>
       </c>
-      <c r="G26" s="7"/>
       <c r="H26" s="6"/>
       <c r="U26" s="1">
         <v>1.7497512683798899</v>
@@ -4554,16 +4622,19 @@
       <c r="B27" s="5"/>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
-        <v>32929</v>
+        <v>32939</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6">
         <v>32854</v>
       </c>
       <c r="F27" s="7">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="G27" s="7">
         <v>75</v>
       </c>
-      <c r="G27" s="7"/>
       <c r="H27" s="6"/>
       <c r="U27" s="1">
         <v>12.7087579765657</v>
@@ -4579,18 +4650,18 @@
       <c r="B28" s="5"/>
       <c r="C28" s="6">
         <f t="shared" si="0"/>
-        <v>32944</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>26</v>
+        <v>32954</v>
       </c>
       <c r="E28" s="6">
         <v>32854</v>
       </c>
       <c r="F28" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G28" s="7">
         <v>90</v>
       </c>
-      <c r="G28" s="7"/>
       <c r="H28" s="6"/>
       <c r="U28" s="1">
         <v>16.912347582510201</v>
@@ -4606,16 +4677,24 @@
       <c r="B29" s="5"/>
       <c r="C29" s="6">
         <f t="shared" si="0"/>
-        <v>32960</v>
+        <v>32970</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="E29" s="6">
         <v>32854</v>
       </c>
       <c r="F29" s="7">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="G29" s="7">
         <v>106</v>
       </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="6"/>
+      <c r="H29" s="7">
+        <v>10</v>
+      </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -4904,7 +4983,7 @@
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="6">
-        <f t="shared" ref="C38:C71" si="1">E38+F38</f>
+        <f t="shared" ref="C38:C71" si="2">E38+F38</f>
         <v>35447</v>
       </c>
       <c r="D38" s="6"/>
@@ -4939,7 +5018,7 @@
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35468</v>
       </c>
       <c r="D39" s="6"/>
@@ -4976,7 +5055,7 @@
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35489</v>
       </c>
       <c r="D40" s="6"/>
@@ -5011,7 +5090,7 @@
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35531</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -5055,7 +5134,7 @@
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35405</v>
       </c>
       <c r="D42" s="6"/>
@@ -5087,7 +5166,7 @@
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35426</v>
       </c>
       <c r="D43" s="6"/>
@@ -5119,7 +5198,7 @@
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35447</v>
       </c>
       <c r="D44" s="6"/>
@@ -5154,7 +5233,7 @@
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35468</v>
       </c>
       <c r="D45" s="6"/>
@@ -5189,7 +5268,7 @@
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35489</v>
       </c>
       <c r="D46" s="6"/>
@@ -5224,7 +5303,7 @@
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35531</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -5269,7 +5348,7 @@
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35405</v>
       </c>
       <c r="D48" s="6"/>
@@ -5301,7 +5380,7 @@
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35426</v>
       </c>
       <c r="D49" s="6"/>
@@ -5333,7 +5412,7 @@
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35447</v>
       </c>
       <c r="D50" s="6"/>
@@ -5368,7 +5447,7 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35468</v>
       </c>
       <c r="D51" s="6"/>
@@ -5403,7 +5482,7 @@
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35489</v>
       </c>
       <c r="D52" s="6"/>
@@ -5438,7 +5517,7 @@
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35531</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -5482,7 +5561,7 @@
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35405</v>
       </c>
       <c r="D54" s="6"/>
@@ -5514,7 +5593,7 @@
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35426</v>
       </c>
       <c r="D55" s="6"/>
@@ -5546,7 +5625,7 @@
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35447</v>
       </c>
       <c r="D56" s="6"/>
@@ -5581,7 +5660,7 @@
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35468</v>
       </c>
       <c r="D57" s="6"/>
@@ -5616,7 +5695,7 @@
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35489</v>
       </c>
       <c r="D58" s="6"/>
@@ -5653,7 +5732,7 @@
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35531</v>
       </c>
       <c r="D59" s="6" t="s">
@@ -5697,7 +5776,7 @@
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35405</v>
       </c>
       <c r="D60" s="6"/>
@@ -5729,7 +5808,7 @@
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35426</v>
       </c>
       <c r="D61" s="6"/>
@@ -5761,7 +5840,7 @@
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35447</v>
       </c>
       <c r="D62" s="6"/>
@@ -5796,7 +5875,7 @@
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35468</v>
       </c>
       <c r="D63" s="6"/>
@@ -5831,7 +5910,7 @@
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35489</v>
       </c>
       <c r="D64" s="6"/>
@@ -5866,7 +5945,7 @@
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35531</v>
       </c>
       <c r="D65" s="6" t="s">
@@ -5911,7 +5990,7 @@
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35776</v>
       </c>
       <c r="D66" s="6"/>
@@ -5919,7 +5998,7 @@
         <v>35741</v>
       </c>
       <c r="F66" s="7">
-        <f t="shared" ref="F66:F85" si="2">H66+G66</f>
+        <f t="shared" ref="F66:F85" si="3">H66+G66</f>
         <v>35</v>
       </c>
       <c r="G66" s="2">
@@ -5941,7 +6020,7 @@
       </c>
       <c r="B67" s="9"/>
       <c r="C67" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35797</v>
       </c>
       <c r="D67" s="6"/>
@@ -5949,7 +6028,7 @@
         <v>35741</v>
       </c>
       <c r="F67" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="G67" s="2">
@@ -5971,7 +6050,7 @@
       </c>
       <c r="B68" s="9"/>
       <c r="C68" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35818</v>
       </c>
       <c r="D68" s="6"/>
@@ -5979,7 +6058,7 @@
         <v>35741</v>
       </c>
       <c r="F68" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="G68" s="2">
@@ -6001,7 +6080,7 @@
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35839</v>
       </c>
       <c r="D69" s="6"/>
@@ -6009,7 +6088,7 @@
         <v>35741</v>
       </c>
       <c r="F69" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="G69" s="2">
@@ -6031,7 +6110,7 @@
       </c>
       <c r="B70" s="9"/>
       <c r="C70" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35860</v>
       </c>
       <c r="D70" s="6"/>
@@ -6039,7 +6118,7 @@
         <v>35741</v>
       </c>
       <c r="F70" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="G70" s="2">
@@ -6061,7 +6140,7 @@
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35881</v>
       </c>
       <c r="D71" s="6"/>
@@ -6069,7 +6148,7 @@
         <v>35741</v>
       </c>
       <c r="F71" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="G71" s="2">
@@ -6101,7 +6180,7 @@
         <v>35741</v>
       </c>
       <c r="F72" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>161</v>
       </c>
       <c r="G72" s="2">
@@ -6139,7 +6218,7 @@
       </c>
       <c r="B73" s="9"/>
       <c r="C73" s="6">
-        <f t="shared" ref="C73:C78" si="3">E73+F73</f>
+        <f t="shared" ref="C73:C78" si="4">E73+F73</f>
         <v>35776</v>
       </c>
       <c r="D73" s="6"/>
@@ -6147,7 +6226,7 @@
         <v>35741</v>
       </c>
       <c r="F73" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="G73" s="2">
@@ -6168,7 +6247,7 @@
       </c>
       <c r="B74" s="9"/>
       <c r="C74" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35797</v>
       </c>
       <c r="D74" s="6"/>
@@ -6176,7 +6255,7 @@
         <v>35741</v>
       </c>
       <c r="F74" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="G74" s="2">
@@ -6197,7 +6276,7 @@
       </c>
       <c r="B75" s="9"/>
       <c r="C75" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35818</v>
       </c>
       <c r="D75" s="6"/>
@@ -6205,7 +6284,7 @@
         <v>35741</v>
       </c>
       <c r="F75" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="G75" s="2">
@@ -6226,7 +6305,7 @@
       </c>
       <c r="B76" s="9"/>
       <c r="C76" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35839</v>
       </c>
       <c r="D76" s="6"/>
@@ -6234,7 +6313,7 @@
         <v>35741</v>
       </c>
       <c r="F76" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="G76" s="2">
@@ -6255,7 +6334,7 @@
       </c>
       <c r="B77" s="9"/>
       <c r="C77" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35860</v>
       </c>
       <c r="D77" s="6"/>
@@ -6263,7 +6342,7 @@
         <v>35741</v>
       </c>
       <c r="F77" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="G77" s="2">
@@ -6284,7 +6363,7 @@
       </c>
       <c r="B78" s="9"/>
       <c r="C78" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35881</v>
       </c>
       <c r="D78" s="6"/>
@@ -6292,7 +6371,7 @@
         <v>35741</v>
       </c>
       <c r="F78" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="G78" s="2">
@@ -6323,7 +6402,7 @@
         <v>35741</v>
       </c>
       <c r="F79" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>161</v>
       </c>
       <c r="G79" s="2">
@@ -6361,7 +6440,7 @@
       </c>
       <c r="B80" s="9"/>
       <c r="C80" s="6">
-        <f t="shared" ref="C80:C85" si="4">E80+F80</f>
+        <f t="shared" ref="C80:C85" si="5">E80+F80</f>
         <v>35776</v>
       </c>
       <c r="D80" s="6"/>
@@ -6369,7 +6448,7 @@
         <v>35741</v>
       </c>
       <c r="F80" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="G80" s="2">
@@ -6390,7 +6469,7 @@
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35797</v>
       </c>
       <c r="D81" s="6"/>
@@ -6398,7 +6477,7 @@
         <v>35741</v>
       </c>
       <c r="F81" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="G81" s="2">
@@ -6419,7 +6498,7 @@
       </c>
       <c r="B82" s="9"/>
       <c r="C82" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35818</v>
       </c>
       <c r="D82" s="6"/>
@@ -6427,7 +6506,7 @@
         <v>35741</v>
       </c>
       <c r="F82" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="G82" s="2">
@@ -6448,7 +6527,7 @@
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35839</v>
       </c>
       <c r="D83" s="6"/>
@@ -6456,7 +6535,7 @@
         <v>35741</v>
       </c>
       <c r="F83" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="G83" s="2">
@@ -6477,7 +6556,7 @@
       </c>
       <c r="B84" s="9"/>
       <c r="C84" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35860</v>
       </c>
       <c r="D84" s="6"/>
@@ -6485,7 +6564,7 @@
         <v>35741</v>
       </c>
       <c r="F84" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="G84" s="2">
@@ -6506,7 +6585,7 @@
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35881</v>
       </c>
       <c r="D85" s="6"/>
@@ -6514,7 +6593,7 @@
         <v>35741</v>
       </c>
       <c r="F85" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="G85" s="2">
@@ -6576,7 +6655,7 @@
       </c>
       <c r="B87" s="9"/>
       <c r="C87" s="6">
-        <f t="shared" ref="C87:C92" si="5">E87+F87</f>
+        <f t="shared" ref="C87:C92" si="6">E87+F87</f>
         <v>35776</v>
       </c>
       <c r="D87" s="6"/>
@@ -6584,7 +6663,7 @@
         <v>35741</v>
       </c>
       <c r="F87" s="7">
-        <f t="shared" ref="F87:F92" si="6">H87+G87</f>
+        <f t="shared" ref="F87:F92" si="7">H87+G87</f>
         <v>35</v>
       </c>
       <c r="G87" s="2">
@@ -6605,7 +6684,7 @@
       </c>
       <c r="B88" s="9"/>
       <c r="C88" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35797</v>
       </c>
       <c r="D88" s="6"/>
@@ -6613,7 +6692,7 @@
         <v>35741</v>
       </c>
       <c r="F88" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
       <c r="G88" s="2">
@@ -6634,7 +6713,7 @@
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35818</v>
       </c>
       <c r="D89" s="6"/>
@@ -6642,7 +6721,7 @@
         <v>35741</v>
       </c>
       <c r="F89" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>77</v>
       </c>
       <c r="G89" s="2">
@@ -6663,7 +6742,7 @@
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35839</v>
       </c>
       <c r="D90" s="6"/>
@@ -6671,7 +6750,7 @@
         <v>35741</v>
       </c>
       <c r="F90" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>98</v>
       </c>
       <c r="G90" s="2">
@@ -6692,7 +6771,7 @@
       </c>
       <c r="B91" s="9"/>
       <c r="C91" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35860</v>
       </c>
       <c r="D91" s="6"/>
@@ -6700,7 +6779,7 @@
         <v>35741</v>
       </c>
       <c r="F91" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>119</v>
       </c>
       <c r="G91" s="2">
@@ -6721,7 +6800,7 @@
       </c>
       <c r="B92" s="9"/>
       <c r="C92" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35881</v>
       </c>
       <c r="D92" s="6"/>
@@ -6729,7 +6808,7 @@
         <v>35741</v>
       </c>
       <c r="F92" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="G92" s="2">
@@ -6750,7 +6829,7 @@
       </c>
       <c r="B93" s="9"/>
       <c r="C93" s="8">
-        <f t="shared" ref="C93:C101" si="7">E93+J93</f>
+        <f t="shared" ref="C93:C101" si="8">E93+J93</f>
         <v>35902</v>
       </c>
       <c r="D93" s="6" t="s">
@@ -6781,7 +6860,7 @@
         <v>343.28169175006798</v>
       </c>
       <c r="AA93" s="1">
-        <f t="shared" ref="AA93:AA101" si="8">T93/Y93</f>
+        <f t="shared" ref="AA93:AA101" si="9">T93/Y93</f>
         <v>0.61517153956727488</v>
       </c>
     </row>
@@ -6791,7 +6870,7 @@
       </c>
       <c r="B94" s="9"/>
       <c r="C94" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35902</v>
       </c>
       <c r="D94" s="6" t="s">
@@ -6822,7 +6901,7 @@
         <v>1047.5702821131399</v>
       </c>
       <c r="AA94" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.5877198616698468</v>
       </c>
     </row>
@@ -6832,7 +6911,7 @@
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35902</v>
       </c>
       <c r="D95" s="6" t="s">
@@ -6863,7 +6942,7 @@
         <v>796.46496972084105</v>
       </c>
       <c r="AA95" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.59785332049875728</v>
       </c>
     </row>
@@ -6873,7 +6952,7 @@
       </c>
       <c r="B96" s="9"/>
       <c r="C96" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35902</v>
       </c>
       <c r="D96" s="6" t="s">
@@ -6904,7 +6983,7 @@
         <v>699.06221414893105</v>
       </c>
       <c r="AA96" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.5966570064180915</v>
       </c>
     </row>
@@ -6914,7 +6993,7 @@
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35902</v>
       </c>
       <c r="D97" s="6" t="s">
@@ -6945,7 +7024,7 @@
         <v>655.12957718011205</v>
       </c>
       <c r="AA97" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.58478450560410777</v>
       </c>
     </row>
@@ -6955,7 +7034,7 @@
       </c>
       <c r="B98" s="9"/>
       <c r="C98" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35902</v>
       </c>
       <c r="D98" s="6" t="s">
@@ -6986,7 +7065,7 @@
         <v>1030.5631638546899</v>
       </c>
       <c r="AA98" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.57435408989559844</v>
       </c>
     </row>
@@ -6996,7 +7075,7 @@
       </c>
       <c r="B99" s="9"/>
       <c r="C99" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35902</v>
       </c>
       <c r="D99" s="6" t="s">
@@ -7027,7 +7106,7 @@
         <v>845.29513434514297</v>
       </c>
       <c r="AA99" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.55432121382614619</v>
       </c>
     </row>
@@ -7037,7 +7116,7 @@
       </c>
       <c r="B100" s="9"/>
       <c r="C100" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35902</v>
       </c>
       <c r="D100" s="6" t="s">
@@ -7068,7 +7147,7 @@
         <v>785.61059731698401</v>
       </c>
       <c r="AA100" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.56902564173601522</v>
       </c>
     </row>
@@ -7078,7 +7157,7 @@
       </c>
       <c r="B101" s="9"/>
       <c r="C101" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35902</v>
       </c>
       <c r="D101" s="6" t="s">
@@ -7109,7 +7188,7 @@
         <v>716.45025122502898</v>
       </c>
       <c r="AA101" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.5415984268554952</v>
       </c>
     </row>
@@ -7119,7 +7198,7 @@
       </c>
       <c r="B102" s="9"/>
       <c r="C102" s="6">
-        <f t="shared" ref="C102:C107" si="9">E102+F102</f>
+        <f t="shared" ref="C102:C107" si="10">E102+F102</f>
         <v>35776</v>
       </c>
       <c r="D102" s="6"/>
@@ -7127,7 +7206,7 @@
         <v>35741</v>
       </c>
       <c r="F102" s="7">
-        <f t="shared" ref="F102:F107" si="10">H102+G102</f>
+        <f t="shared" ref="F102:F107" si="11">H102+G102</f>
         <v>35</v>
       </c>
       <c r="G102" s="2">
@@ -7151,7 +7230,7 @@
       </c>
       <c r="B103" s="9"/>
       <c r="C103" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>35797</v>
       </c>
       <c r="D103" s="6"/>
@@ -7159,7 +7238,7 @@
         <v>35741</v>
       </c>
       <c r="F103" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>56</v>
       </c>
       <c r="G103" s="2">
@@ -7183,7 +7262,7 @@
       </c>
       <c r="B104" s="9"/>
       <c r="C104" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>35818</v>
       </c>
       <c r="D104" s="6"/>
@@ -7191,7 +7270,7 @@
         <v>35741</v>
       </c>
       <c r="F104" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>77</v>
       </c>
       <c r="G104" s="2">
@@ -7215,7 +7294,7 @@
       </c>
       <c r="B105" s="9"/>
       <c r="C105" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>35839</v>
       </c>
       <c r="D105" s="6"/>
@@ -7223,7 +7302,7 @@
         <v>35741</v>
       </c>
       <c r="F105" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>98</v>
       </c>
       <c r="G105" s="2">
@@ -7247,7 +7326,7 @@
       </c>
       <c r="B106" s="9"/>
       <c r="C106" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>35860</v>
       </c>
       <c r="D106" s="6"/>
@@ -7255,7 +7334,7 @@
         <v>35741</v>
       </c>
       <c r="F106" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>119</v>
       </c>
       <c r="G106" s="2">
@@ -7279,7 +7358,7 @@
       </c>
       <c r="B107" s="9"/>
       <c r="C107" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>35881</v>
       </c>
       <c r="D107" s="6"/>
@@ -7287,7 +7366,7 @@
         <v>35741</v>
       </c>
       <c r="F107" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>140</v>
       </c>
       <c r="G107" s="2">
@@ -7305,7 +7384,7 @@
         <v>1124.9410322956101</v>
       </c>
       <c r="AA107" s="1">
-        <f t="shared" ref="AA107:AA115" si="11">T107/Y107</f>
+        <f t="shared" ref="AA107:AA115" si="12">T107/Y107</f>
         <v>0.5164687627891642</v>
       </c>
     </row>
@@ -7346,7 +7425,7 @@
         <v>1297.83741710808</v>
       </c>
       <c r="AA108" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.54760057573932719</v>
       </c>
     </row>
@@ -7387,7 +7466,7 @@
         <v>1135.43192825251</v>
       </c>
       <c r="AA109" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.55106873051835448</v>
       </c>
     </row>
@@ -7428,7 +7507,7 @@
         <v>1009.9101083416</v>
       </c>
       <c r="AA110" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.54152216496102545</v>
       </c>
     </row>
@@ -7469,7 +7548,7 @@
         <v>859.16057930755699</v>
       </c>
       <c r="AA111" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.52004526213321234</v>
       </c>
     </row>
@@ -7500,7 +7579,7 @@
         <v>1261</v>
       </c>
       <c r="AA112" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.52101506740682002</v>
       </c>
     </row>
@@ -7531,7 +7610,7 @@
         <v>1539</v>
       </c>
       <c r="AA113" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.41585445094217022</v>
       </c>
     </row>
@@ -7562,7 +7641,7 @@
         <v>1556</v>
       </c>
       <c r="AA114" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.41902313624678661</v>
       </c>
     </row>
@@ -7594,7 +7673,7 @@
         <v>1619</v>
       </c>
       <c r="AA115" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.35083384805435452</v>
       </c>
     </row>
@@ -7620,7 +7699,7 @@
         <v>53</v>
       </c>
       <c r="C117" s="8">
-        <f t="shared" ref="C117:C143" si="12">DATE(1981,12,10)+F117+7</f>
+        <f t="shared" ref="C117:C143" si="13">DATE(1981,12,10)+F117+7</f>
         <v>29937</v>
       </c>
       <c r="E117" s="8"/>
@@ -7637,7 +7716,7 @@
         <v>53</v>
       </c>
       <c r="C118" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E118" s="8"/>
@@ -7654,7 +7733,7 @@
         <v>53</v>
       </c>
       <c r="C119" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E119" s="8"/>
@@ -7671,7 +7750,7 @@
         <v>53</v>
       </c>
       <c r="C120" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E120" s="8"/>
@@ -7688,7 +7767,7 @@
         <v>53</v>
       </c>
       <c r="C121" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E121" s="8"/>
@@ -7705,7 +7784,7 @@
         <v>53</v>
       </c>
       <c r="C122" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E122" s="8"/>
@@ -7722,7 +7801,7 @@
         <v>54</v>
       </c>
       <c r="C123" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E123" s="8"/>
@@ -7739,7 +7818,7 @@
         <v>54</v>
       </c>
       <c r="C124" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E124" s="8"/>
@@ -7756,7 +7835,7 @@
         <v>54</v>
       </c>
       <c r="C125" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E125" s="8"/>
@@ -7773,7 +7852,7 @@
         <v>54</v>
       </c>
       <c r="C126" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E126" s="8"/>
@@ -7790,7 +7869,7 @@
         <v>54</v>
       </c>
       <c r="C127" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E127" s="8"/>
@@ -7807,7 +7886,7 @@
         <v>54</v>
       </c>
       <c r="C128" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E128" s="8"/>
@@ -7824,7 +7903,7 @@
         <v>54</v>
       </c>
       <c r="C129" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E129" s="8"/>
@@ -7841,7 +7920,7 @@
         <v>55</v>
       </c>
       <c r="C130" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E130" s="8"/>
@@ -7858,7 +7937,7 @@
         <v>55</v>
       </c>
       <c r="C131" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E131" s="8"/>
@@ -7875,7 +7954,7 @@
         <v>55</v>
       </c>
       <c r="C132" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E132" s="8"/>
@@ -7892,7 +7971,7 @@
         <v>55</v>
       </c>
       <c r="C133" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E133" s="8"/>
@@ -7909,7 +7988,7 @@
         <v>55</v>
       </c>
       <c r="C134" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E134" s="8"/>
@@ -7926,7 +8005,7 @@
         <v>55</v>
       </c>
       <c r="C135" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E135" s="8"/>
@@ -7943,7 +8022,7 @@
         <v>55</v>
       </c>
       <c r="C136" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E136" s="8"/>
@@ -7960,7 +8039,7 @@
         <v>56</v>
       </c>
       <c r="C137" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E137" s="8"/>
@@ -7977,7 +8056,7 @@
         <v>56</v>
       </c>
       <c r="C138" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E138" s="8"/>
@@ -7994,7 +8073,7 @@
         <v>56</v>
       </c>
       <c r="C139" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E139" s="8"/>
@@ -8011,7 +8090,7 @@
         <v>56</v>
       </c>
       <c r="C140" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E140" s="8"/>
@@ -8028,7 +8107,7 @@
         <v>56</v>
       </c>
       <c r="C141" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E141" s="8"/>
@@ -8045,7 +8124,7 @@
         <v>56</v>
       </c>
       <c r="C142" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E142" s="8"/>
@@ -8062,7 +8141,7 @@
         <v>56</v>
       </c>
       <c r="C143" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29937</v>
       </c>
       <c r="E143" s="8"/>
@@ -8094,7 +8173,7 @@
         <v>0.33</v>
       </c>
       <c r="N144" s="1">
-        <f t="shared" ref="N144:N173" si="13">M144/R144</f>
+        <f t="shared" ref="N144:N173" si="14">M144/R144</f>
         <v>2.4699999999999958E-2</v>
       </c>
       <c r="R144" s="1">
@@ -8130,7 +8209,7 @@
         <v>1.06</v>
       </c>
       <c r="N145" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.12E-2</v>
       </c>
       <c r="R145" s="1">
@@ -8167,7 +8246,7 @@
         <v>3.64</v>
       </c>
       <c r="N146" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.6999999999999962E-2</v>
       </c>
       <c r="R146" s="1">
@@ -8203,7 +8282,7 @@
         <v>5.7</v>
       </c>
       <c r="N147" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.6399999999999989E-2</v>
       </c>
       <c r="R147" s="1">
@@ -8239,7 +8318,7 @@
         <v>7.03</v>
       </c>
       <c r="N148" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.5400000000000006E-2</v>
       </c>
       <c r="R148" s="1">
@@ -8285,7 +8364,7 @@
         <v>5.85</v>
       </c>
       <c r="N149" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.1499999999999995E-2</v>
       </c>
       <c r="R149" s="1">
@@ -8325,7 +8404,7 @@
         <v>0.71</v>
       </c>
       <c r="N150" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.0699999999999988E-2</v>
       </c>
       <c r="R150" s="1">
@@ -8363,7 +8442,7 @@
         <v>1.43</v>
       </c>
       <c r="N151" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.8299999999999968E-2</v>
       </c>
       <c r="R151" s="1">
@@ -8401,7 +8480,7 @@
         <v>4.53</v>
       </c>
       <c r="N152" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.9300000000000041E-2</v>
       </c>
       <c r="R152" s="1">
@@ -8440,7 +8519,7 @@
         <v>7.77</v>
       </c>
       <c r="N153" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.6899999999999966E-2</v>
       </c>
       <c r="R153" s="1">
@@ -8479,7 +8558,7 @@
         <v>6.14</v>
       </c>
       <c r="N154" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.2700000000000026E-2</v>
       </c>
       <c r="R154" s="1">
@@ -8527,7 +8606,7 @@
         <v>3.12</v>
       </c>
       <c r="N155" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.1399999999999926E-2</v>
       </c>
       <c r="R155" s="1">
@@ -8568,7 +8647,7 @@
         <v>0.49</v>
       </c>
       <c r="N156" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.7699999999999961E-2</v>
       </c>
       <c r="R156" s="1">
@@ -8604,7 +8683,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="N157" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.6499999999999985E-2</v>
       </c>
       <c r="R157" s="1">
@@ -8640,7 +8719,7 @@
         <v>2.93</v>
       </c>
       <c r="N158" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.3099999999999971E-2</v>
       </c>
       <c r="R158" s="1">
@@ -8677,7 +8756,7 @@
         <v>4.28</v>
       </c>
       <c r="N159" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.9900000000000011E-2</v>
       </c>
       <c r="R159" s="1">
@@ -8715,7 +8794,7 @@
         <v>4.7699999999999996</v>
       </c>
       <c r="N160" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.9300000000000036E-2</v>
       </c>
       <c r="R160" s="1">
@@ -8759,7 +8838,7 @@
         <v>4.3099999999999996</v>
       </c>
       <c r="N161" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.7200000000000014E-2</v>
       </c>
       <c r="R161" s="1">
@@ -8800,7 +8879,7 @@
         <v>0.36</v>
       </c>
       <c r="N162" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.0900000000000007E-2</v>
       </c>
       <c r="R162" s="1">
@@ -8837,7 +8916,7 @@
         <v>1.19</v>
       </c>
       <c r="N163" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.5599999999999998E-2</v>
       </c>
       <c r="R163" s="1">
@@ -8874,7 +8953,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="N164" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.9499999999999979E-2</v>
       </c>
       <c r="R164" s="1">
@@ -8911,7 +8990,7 @@
         <v>2.98</v>
       </c>
       <c r="N165" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.6800000000000034E-2</v>
       </c>
       <c r="R165" s="1">
@@ -8947,7 +9026,7 @@
         <v>3.38</v>
       </c>
       <c r="N166" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.6399999999999981E-2</v>
       </c>
       <c r="R166" s="1">
@@ -8994,7 +9073,7 @@
         <v>2.73</v>
       </c>
       <c r="N167" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.6699999999999954E-2</v>
       </c>
       <c r="R167" s="1">
@@ -9034,7 +9113,7 @@
         <v>0.18</v>
       </c>
       <c r="N168" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.3200000000000005E-2</v>
       </c>
       <c r="R168" s="1">
@@ -9070,7 +9149,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N169" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.2100000000000002E-2</v>
       </c>
       <c r="R169" s="1">
@@ -9106,7 +9185,7 @@
         <v>1.91</v>
       </c>
       <c r="N170" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.8199999999999987E-2</v>
       </c>
       <c r="R170" s="1">
@@ -9142,7 +9221,7 @@
         <v>2.44</v>
       </c>
       <c r="N171" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.6900000000000009E-2</v>
       </c>
       <c r="R171" s="1">
@@ -9179,7 +9258,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="N172" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.5200000000000021E-2</v>
       </c>
       <c r="R172" s="1">
@@ -9226,7 +9305,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="N173" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.7000000000000029E-2</v>
       </c>
       <c r="R173" s="1">
@@ -9254,7 +9333,7 @@
         <v>68</v>
       </c>
       <c r="C174" s="6">
-        <f t="shared" ref="C174:C221" si="14">E174+F174</f>
+        <f t="shared" ref="C174:C221" si="15">E174+F174</f>
         <v>31023</v>
       </c>
       <c r="D174" s="6"/>
@@ -9286,7 +9365,7 @@
         <v>68</v>
       </c>
       <c r="C175" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31037</v>
       </c>
       <c r="E175" s="6">
@@ -9317,7 +9396,7 @@
         <v>68</v>
       </c>
       <c r="C176" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31051</v>
       </c>
       <c r="E176" s="6">
@@ -9348,7 +9427,7 @@
         <v>68</v>
       </c>
       <c r="C177" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31064</v>
       </c>
       <c r="E177" s="6">
@@ -9379,7 +9458,7 @@
         <v>68</v>
       </c>
       <c r="C178" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31078</v>
       </c>
       <c r="D178" s="13"/>
@@ -9408,7 +9487,7 @@
         <v>68</v>
       </c>
       <c r="C179" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31091</v>
       </c>
       <c r="D179" s="13"/>
@@ -9438,7 +9517,7 @@
         <v>68</v>
       </c>
       <c r="C180" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31104</v>
       </c>
       <c r="D180" s="13"/>
@@ -9467,7 +9546,7 @@
         <v>68</v>
       </c>
       <c r="C181" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31118</v>
       </c>
       <c r="D181" s="6" t="s">
@@ -9505,7 +9584,7 @@
         <v>68</v>
       </c>
       <c r="C182" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31023</v>
       </c>
       <c r="D182" s="6"/>
@@ -9534,7 +9613,7 @@
         <v>68</v>
       </c>
       <c r="C183" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31037</v>
       </c>
       <c r="E183" s="6">
@@ -9562,7 +9641,7 @@
         <v>68</v>
       </c>
       <c r="C184" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31051</v>
       </c>
       <c r="E184" s="6">
@@ -9590,7 +9669,7 @@
         <v>68</v>
       </c>
       <c r="C185" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31064</v>
       </c>
       <c r="E185" s="6">
@@ -9618,7 +9697,7 @@
         <v>68</v>
       </c>
       <c r="C186" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31078</v>
       </c>
       <c r="D186" s="13"/>
@@ -9648,7 +9727,7 @@
         <v>68</v>
       </c>
       <c r="C187" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31091</v>
       </c>
       <c r="D187" s="13"/>
@@ -9677,7 +9756,7 @@
         <v>68</v>
       </c>
       <c r="C188" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31104</v>
       </c>
       <c r="D188" s="13"/>
@@ -9706,7 +9785,7 @@
         <v>68</v>
       </c>
       <c r="C189" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31118</v>
       </c>
       <c r="D189" s="6" t="s">
@@ -9744,7 +9823,7 @@
         <v>71</v>
       </c>
       <c r="C190" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31056</v>
       </c>
       <c r="D190" s="13"/>
@@ -9773,7 +9852,7 @@
         <v>71</v>
       </c>
       <c r="C191" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31070</v>
       </c>
       <c r="D191" s="13"/>
@@ -9802,7 +9881,7 @@
         <v>71</v>
       </c>
       <c r="C192" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31084</v>
       </c>
       <c r="D192" s="13"/>
@@ -9831,7 +9910,7 @@
         <v>71</v>
       </c>
       <c r="C193" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31104</v>
       </c>
       <c r="D193" s="13"/>
@@ -9861,7 +9940,7 @@
         <v>71</v>
       </c>
       <c r="C194" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31118</v>
       </c>
       <c r="D194" s="13"/>
@@ -9890,7 +9969,7 @@
         <v>71</v>
       </c>
       <c r="C195" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31134</v>
       </c>
       <c r="D195" s="13"/>
@@ -9919,7 +9998,7 @@
         <v>71</v>
       </c>
       <c r="C196" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31148</v>
       </c>
       <c r="D196" s="13"/>
@@ -9948,7 +10027,7 @@
         <v>71</v>
       </c>
       <c r="C197" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31161</v>
       </c>
       <c r="D197" s="6" t="s">
@@ -9986,7 +10065,7 @@
         <v>71</v>
       </c>
       <c r="C198" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31056</v>
       </c>
       <c r="D198" s="13"/>
@@ -10015,7 +10094,7 @@
         <v>71</v>
       </c>
       <c r="C199" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31070</v>
       </c>
       <c r="D199" s="13"/>
@@ -10044,7 +10123,7 @@
         <v>71</v>
       </c>
       <c r="C200" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31084</v>
       </c>
       <c r="D200" s="13"/>
@@ -10074,7 +10153,7 @@
         <v>71</v>
       </c>
       <c r="C201" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31104</v>
       </c>
       <c r="D201" s="13"/>
@@ -10103,7 +10182,7 @@
         <v>71</v>
       </c>
       <c r="C202" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31118</v>
       </c>
       <c r="D202" s="13"/>
@@ -10132,7 +10211,7 @@
         <v>71</v>
       </c>
       <c r="C203" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31134</v>
       </c>
       <c r="D203" s="13"/>
@@ -10161,7 +10240,7 @@
         <v>71</v>
       </c>
       <c r="C204" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31148</v>
       </c>
       <c r="D204" s="13"/>
@@ -10190,7 +10269,7 @@
         <v>71</v>
       </c>
       <c r="C205" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31161</v>
       </c>
       <c r="D205" s="6" t="s">
@@ -10228,7 +10307,7 @@
         <v>74</v>
       </c>
       <c r="C206" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31105</v>
       </c>
       <c r="D206" s="13"/>
@@ -10257,7 +10336,7 @@
         <v>74</v>
       </c>
       <c r="C207" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31113</v>
       </c>
       <c r="D207" s="13"/>
@@ -10287,7 +10366,7 @@
         <v>74</v>
       </c>
       <c r="C208" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31127</v>
       </c>
       <c r="D208" s="13"/>
@@ -10316,7 +10395,7 @@
         <v>74</v>
       </c>
       <c r="C209" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31141</v>
       </c>
       <c r="D209" s="13"/>
@@ -10345,7 +10424,7 @@
         <v>74</v>
       </c>
       <c r="C210" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31162</v>
       </c>
       <c r="D210" s="13"/>
@@ -10374,7 +10453,7 @@
         <v>74</v>
       </c>
       <c r="C211" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31177</v>
       </c>
       <c r="D211" s="13"/>
@@ -10403,7 +10482,7 @@
         <v>74</v>
       </c>
       <c r="C212" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31189</v>
       </c>
       <c r="D212" s="13"/>
@@ -10432,7 +10511,7 @@
         <v>74</v>
       </c>
       <c r="C213" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31195</v>
       </c>
       <c r="D213" s="6" t="s">
@@ -10470,7 +10549,7 @@
         <v>74</v>
       </c>
       <c r="C214" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31105</v>
       </c>
       <c r="D214" s="13"/>
@@ -10500,7 +10579,7 @@
         <v>74</v>
       </c>
       <c r="C215" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31113</v>
       </c>
       <c r="D215" s="13"/>
@@ -10529,7 +10608,7 @@
         <v>74</v>
       </c>
       <c r="C216" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31127</v>
       </c>
       <c r="D216" s="13"/>
@@ -10558,7 +10637,7 @@
         <v>74</v>
       </c>
       <c r="C217" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31141</v>
       </c>
       <c r="D217" s="13"/>
@@ -10587,7 +10666,7 @@
         <v>74</v>
       </c>
       <c r="C218" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31162</v>
       </c>
       <c r="D218" s="13"/>
@@ -10616,7 +10695,7 @@
         <v>74</v>
       </c>
       <c r="C219" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31177</v>
       </c>
       <c r="D219" s="13"/>
@@ -10645,7 +10724,7 @@
         <v>74</v>
       </c>
       <c r="C220" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31189</v>
       </c>
       <c r="D220" s="13"/>
@@ -10674,7 +10753,7 @@
         <v>74</v>
       </c>
       <c r="C221" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31195</v>
       </c>
       <c r="D221" s="6" t="s">
@@ -11438,7 +11517,7 @@
         <v>152</v>
       </c>
       <c r="C265" s="23">
-        <f t="shared" ref="C265:C275" si="15">DATE(1988,4,28)+F265</f>
+        <f t="shared" ref="C265:C275" si="16">DATE(1988,4,28)+F265</f>
         <v>32302</v>
       </c>
       <c r="F265" s="2">
@@ -11456,7 +11535,7 @@
         <v>0.83718759722078295</v>
       </c>
       <c r="N265" s="1">
-        <f t="shared" ref="N265:N275" si="16">M265/P265</f>
+        <f t="shared" ref="N265:N275" si="17">M265/P265</f>
         <v>2.1493181582495167E-2</v>
       </c>
       <c r="P265" s="1">
@@ -11472,14 +11551,14 @@
         <v>1.19006321307415</v>
       </c>
       <c r="Y265" s="1">
-        <f t="shared" ref="Y265:Y275" si="17">T265+S265+R265</f>
+        <f t="shared" ref="Y265:Y275" si="18">T265+S265+R265</f>
         <v>78.916884278578848</v>
       </c>
       <c r="AB265">
         <v>164.784053156146</v>
       </c>
       <c r="AC265">
-        <f t="shared" ref="AC265:AC275" si="18">M265/L265</f>
+        <f t="shared" ref="AC265:AC275" si="19">M265/L265</f>
         <v>1.0972662379767062E-3</v>
       </c>
     </row>
@@ -11488,11 +11567,11 @@
         <v>152</v>
       </c>
       <c r="C266" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32309</v>
       </c>
       <c r="F266" s="2">
-        <f t="shared" ref="F266:F275" si="19">F265+7</f>
+        <f t="shared" ref="F266:F275" si="20">F265+7</f>
         <v>48</v>
       </c>
       <c r="I266" s="8"/>
@@ -11506,7 +11585,7 @@
         <v>1.4875557399149599</v>
       </c>
       <c r="N266" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.2065410142071924E-2</v>
       </c>
       <c r="P266" s="1">
@@ -11522,14 +11601,14 @@
         <v>1.07442954054886</v>
       </c>
       <c r="Y266" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>158.28607824497425</v>
       </c>
       <c r="AB266">
         <v>188.039867109634</v>
       </c>
       <c r="AC266">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.5261624661373396E-3</v>
       </c>
     </row>
@@ -11538,11 +11617,11 @@
         <v>152</v>
       </c>
       <c r="C267" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32316</v>
       </c>
       <c r="F267" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>55</v>
       </c>
       <c r="I267" s="8"/>
@@ -11556,7 +11635,7 @@
         <v>2.0486363164990098</v>
       </c>
       <c r="N267" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.8992565850876386E-2</v>
       </c>
       <c r="P267" s="1">
@@ -11572,14 +11651,14 @@
         <v>2.7944804193646098</v>
       </c>
       <c r="Y267" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>237.1902612035866</v>
       </c>
       <c r="AB267">
         <v>264.45182724252402</v>
       </c>
       <c r="AC267">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.466186993348443E-3</v>
       </c>
     </row>
@@ -11588,11 +11667,11 @@
         <v>152</v>
       </c>
       <c r="C268" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32323</v>
       </c>
       <c r="F268" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>62</v>
       </c>
       <c r="I268" s="8"/>
@@ -11606,7 +11685,7 @@
         <v>3.0153997718552299</v>
       </c>
       <c r="N268" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.7351546100977347E-2</v>
       </c>
       <c r="P268" s="1">
@@ -11622,14 +11701,14 @@
         <v>6.3116712920134397</v>
       </c>
       <c r="Y268" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>416.82913670514347</v>
       </c>
       <c r="AB268">
         <v>332.55813953488303</v>
       </c>
       <c r="AC268">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.3974929574937867E-3</v>
       </c>
     </row>
@@ -11638,11 +11717,11 @@
         <v>152</v>
       </c>
       <c r="C269" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32330</v>
       </c>
       <c r="F269" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>69</v>
       </c>
       <c r="I269" s="8"/>
@@ -11656,7 +11735,7 @@
         <v>2.4253862905734702</v>
       </c>
       <c r="N269" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.0236816861972495E-2</v>
       </c>
       <c r="P269" s="1">
@@ -11672,14 +11751,14 @@
         <v>13.447232500770699</v>
       </c>
       <c r="Y269" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>304.7259911952587</v>
       </c>
       <c r="AB269">
         <v>395.68106312292298</v>
       </c>
       <c r="AC269">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.9394573416874794E-3</v>
       </c>
     </row>
@@ -11688,11 +11767,11 @@
         <v>152</v>
       </c>
       <c r="C270" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32337</v>
       </c>
       <c r="F270" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>76</v>
       </c>
       <c r="I270" s="8"/>
@@ -11702,11 +11781,11 @@
         <v>152</v>
       </c>
       <c r="C271" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32344</v>
       </c>
       <c r="F271" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>83</v>
       </c>
       <c r="I271" s="8"/>
@@ -11720,7 +11799,7 @@
         <v>4.1557606553976996</v>
       </c>
       <c r="N271" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.7229628804210972E-2</v>
       </c>
       <c r="P271" s="1">
@@ -11736,14 +11815,14 @@
         <v>129.186902559358</v>
       </c>
       <c r="Y271" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>782.63030239119996</v>
       </c>
       <c r="AB271">
         <v>520.26578073089604</v>
       </c>
       <c r="AC271">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.2927374071790795E-3</v>
       </c>
     </row>
@@ -11752,11 +11831,11 @@
         <v>152</v>
       </c>
       <c r="C272" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32351</v>
       </c>
       <c r="F272" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>90</v>
       </c>
       <c r="I272" s="8"/>
@@ -11770,7 +11849,7 @@
         <v>3.6783677278855098</v>
       </c>
       <c r="N272" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.2991060626262332E-2</v>
       </c>
       <c r="P272" s="1">
@@ -11786,14 +11865,14 @@
         <v>158.06159420289799</v>
       </c>
       <c r="Y272" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>916.71786570026006</v>
       </c>
       <c r="AB272">
         <v>453.82059800664399</v>
       </c>
       <c r="AC272">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.0702612659552121E-3</v>
       </c>
     </row>
@@ -11802,11 +11881,11 @@
         <v>152</v>
       </c>
       <c r="C273" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32358</v>
       </c>
       <c r="F273" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>97</v>
       </c>
       <c r="I273" s="8"/>
@@ -11820,7 +11899,7 @@
         <v>5.3219433786166102</v>
       </c>
       <c r="N273" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.6599986940311187E-2</v>
       </c>
       <c r="P273" s="1">
@@ -11836,14 +11915,14 @@
         <v>299.26476256552502</v>
       </c>
       <c r="Y273" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1066.8027890120579</v>
       </c>
       <c r="AB273">
         <v>463.78737541528204</v>
       </c>
       <c r="AC273">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.4932277493432148E-3</v>
       </c>
     </row>
@@ -11852,11 +11931,11 @@
         <v>152</v>
       </c>
       <c r="C274" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32365</v>
       </c>
       <c r="F274" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>104</v>
       </c>
       <c r="I274" s="8"/>
@@ -11870,7 +11949,7 @@
         <v>4.9798817795291903</v>
       </c>
       <c r="N274" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.6873457298658558E-2</v>
       </c>
       <c r="P274" s="1">
@@ -11886,14 +11965,14 @@
         <v>313.646700585877</v>
       </c>
       <c r="Y274" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1074.0839091771779</v>
       </c>
       <c r="AB274">
         <v>417.27574750830502</v>
       </c>
       <c r="AC274">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.3226499235756053E-3</v>
       </c>
     </row>
@@ -11902,14 +11981,14 @@
         <v>152</v>
       </c>
       <c r="C275" s="23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32372</v>
       </c>
       <c r="D275" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F275" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>111</v>
       </c>
       <c r="I275" s="8"/>
@@ -11923,7 +12002,7 @@
         <v>5.1565902727367003</v>
       </c>
       <c r="N275" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.5096596522156794E-2</v>
       </c>
       <c r="P275" s="1">
@@ -11939,14 +12018,14 @@
         <v>409.540741597286</v>
       </c>
       <c r="Y275" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1296.011734488824</v>
       </c>
       <c r="AB275">
         <v>427.24252491694301</v>
       </c>
       <c r="AC275">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.4088548708033129E-3</v>
       </c>
     </row>
@@ -11980,7 +12059,7 @@
         <v>154</v>
       </c>
       <c r="C277" s="8">
-        <f t="shared" ref="C277:C294" si="20">DATE(1990,5,15)+G277+6</f>
+        <f t="shared" ref="C277:C294" si="21">DATE(1990,5,15)+G277+6</f>
         <v>33037</v>
       </c>
       <c r="G277" s="2">
@@ -12005,7 +12084,7 @@
         <v>154</v>
       </c>
       <c r="C278" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33044</v>
       </c>
       <c r="G278" s="2">
@@ -12030,7 +12109,7 @@
         <v>154</v>
       </c>
       <c r="C279" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33051</v>
       </c>
       <c r="G279" s="2">
@@ -12055,7 +12134,7 @@
         <v>154</v>
       </c>
       <c r="C280" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33058</v>
       </c>
       <c r="G280" s="2">
@@ -12080,7 +12159,7 @@
         <v>154</v>
       </c>
       <c r="C281" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33065</v>
       </c>
       <c r="G281" s="2">
@@ -12105,7 +12184,7 @@
         <v>154</v>
       </c>
       <c r="C282" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33072</v>
       </c>
       <c r="G282" s="2">
@@ -12130,7 +12209,7 @@
         <v>154</v>
       </c>
       <c r="C283" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33079</v>
       </c>
       <c r="G283" s="2">
@@ -12155,7 +12234,7 @@
         <v>154</v>
       </c>
       <c r="C284" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33086</v>
       </c>
       <c r="G284" s="2">
@@ -12180,7 +12259,7 @@
         <v>154</v>
       </c>
       <c r="C285" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33093</v>
       </c>
       <c r="G285" s="2">
@@ -12205,7 +12284,7 @@
         <v>154</v>
       </c>
       <c r="C286" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33100</v>
       </c>
       <c r="G286" s="2">
@@ -12230,7 +12309,7 @@
         <v>154</v>
       </c>
       <c r="C287" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33107</v>
       </c>
       <c r="G287" s="2">
@@ -12255,7 +12334,7 @@
         <v>154</v>
       </c>
       <c r="C288" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33114</v>
       </c>
       <c r="G288" s="2">
@@ -12280,7 +12359,7 @@
         <v>154</v>
       </c>
       <c r="C289" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33121</v>
       </c>
       <c r="G289" s="2">
@@ -12305,7 +12384,7 @@
         <v>154</v>
       </c>
       <c r="C290" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33128</v>
       </c>
       <c r="G290" s="2">
@@ -12330,7 +12409,7 @@
         <v>154</v>
       </c>
       <c r="C291" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33135</v>
       </c>
       <c r="G291" s="2">
@@ -12355,7 +12434,7 @@
         <v>154</v>
       </c>
       <c r="C292" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33142</v>
       </c>
       <c r="G292" s="2">
@@ -12380,7 +12459,7 @@
         <v>154</v>
       </c>
       <c r="C293" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33149</v>
       </c>
       <c r="G293" s="2">
@@ -12405,7 +12484,7 @@
         <v>154</v>
       </c>
       <c r="C294" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33156</v>
       </c>
       <c r="D294" s="6" t="s">
@@ -12455,7 +12534,7 @@
         <v>53</v>
       </c>
       <c r="C296" s="8">
-        <f t="shared" ref="C296:C327" si="21">DATE(1981,12,10)+F296</f>
+        <f t="shared" ref="C296:C320" si="22">DATE(1981,12,10)+F296</f>
         <v>29959</v>
       </c>
       <c r="F296" s="2">
@@ -12477,7 +12556,7 @@
         <v>53</v>
       </c>
       <c r="C297" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29966</v>
       </c>
       <c r="F297" s="2">
@@ -12499,7 +12578,7 @@
         <v>53</v>
       </c>
       <c r="C298" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29973</v>
       </c>
       <c r="F298" s="2">
@@ -12521,7 +12600,7 @@
         <v>53</v>
       </c>
       <c r="C299" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29980</v>
       </c>
       <c r="F299" s="2">
@@ -12543,7 +12622,7 @@
         <v>53</v>
       </c>
       <c r="C300" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29987</v>
       </c>
       <c r="F300" s="2">
@@ -12565,7 +12644,7 @@
         <v>53</v>
       </c>
       <c r="C301" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29994</v>
       </c>
       <c r="F301" s="2">
@@ -12587,7 +12666,7 @@
         <v>53</v>
       </c>
       <c r="C302" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30008</v>
       </c>
       <c r="F302" s="2">
@@ -12609,7 +12688,7 @@
         <v>53</v>
       </c>
       <c r="C303" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30022</v>
       </c>
       <c r="F303" s="2">
@@ -12631,7 +12710,7 @@
         <v>53</v>
       </c>
       <c r="C304" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30029</v>
       </c>
       <c r="F304" s="2">
@@ -12653,7 +12732,7 @@
         <v>53</v>
       </c>
       <c r="C305" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30036</v>
       </c>
       <c r="F305" s="2">
@@ -12672,7 +12751,7 @@
         <v>53</v>
       </c>
       <c r="C306" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30043</v>
       </c>
       <c r="F306" s="2">
@@ -12691,7 +12770,7 @@
         <v>53</v>
       </c>
       <c r="C307" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30050</v>
       </c>
       <c r="F307" s="2">
@@ -12710,7 +12789,7 @@
         <v>54</v>
       </c>
       <c r="C308" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29952</v>
       </c>
       <c r="F308" s="2">
@@ -12732,7 +12811,7 @@
         <v>54</v>
       </c>
       <c r="C309" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29959</v>
       </c>
       <c r="F309" s="2">
@@ -12754,7 +12833,7 @@
         <v>54</v>
       </c>
       <c r="C310" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29966</v>
       </c>
       <c r="F310" s="2">
@@ -12776,7 +12855,7 @@
         <v>54</v>
       </c>
       <c r="C311" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29973</v>
       </c>
       <c r="F311" s="2">
@@ -12798,7 +12877,7 @@
         <v>54</v>
       </c>
       <c r="C312" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29980</v>
       </c>
       <c r="F312" s="2">
@@ -12820,7 +12899,7 @@
         <v>54</v>
       </c>
       <c r="C313" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29987</v>
       </c>
       <c r="F313" s="2">
@@ -12842,7 +12921,7 @@
         <v>54</v>
       </c>
       <c r="C314" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>29994</v>
       </c>
       <c r="F314" s="2">
@@ -12864,7 +12943,7 @@
         <v>54</v>
       </c>
       <c r="C315" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30008</v>
       </c>
       <c r="F315" s="2">
@@ -12886,7 +12965,7 @@
         <v>54</v>
       </c>
       <c r="C316" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30022</v>
       </c>
       <c r="F316" s="2">
@@ -12908,7 +12987,7 @@
         <v>54</v>
       </c>
       <c r="C317" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30029</v>
       </c>
       <c r="F317" s="2">
@@ -12930,7 +13009,7 @@
         <v>54</v>
       </c>
       <c r="C318" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30036</v>
       </c>
       <c r="F318" s="2">
@@ -12949,7 +13028,7 @@
         <v>54</v>
       </c>
       <c r="C319" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30043</v>
       </c>
       <c r="F319" s="2">
@@ -12968,7 +13047,7 @@
         <v>54</v>
       </c>
       <c r="C320" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>30050</v>
       </c>
       <c r="F320" s="2">
@@ -12988,9 +13067,13 @@
       </c>
       <c r="C321" s="24">
         <f>DATE(1989,11,24)+F321</f>
-        <v>32873</v>
+        <v>32884</v>
       </c>
       <c r="F321" s="2">
+        <f>G321+11</f>
+        <v>48</v>
+      </c>
+      <c r="G321" s="2">
         <v>37</v>
       </c>
       <c r="T321" s="1">
@@ -13005,10 +13088,14 @@
         <v>156</v>
       </c>
       <c r="C322" s="24">
-        <f t="shared" ref="C322:C340" si="22">DATE(1989,11,24)+F322</f>
-        <v>32887</v>
+        <f t="shared" ref="C322:C340" si="23">DATE(1989,11,24)+F322</f>
+        <v>32898</v>
       </c>
       <c r="F322" s="2">
+        <f t="shared" ref="F322:F340" si="24">G322+11</f>
+        <v>62</v>
+      </c>
+      <c r="G322" s="2">
         <v>51</v>
       </c>
       <c r="T322" s="1">
@@ -13023,10 +13110,14 @@
         <v>156</v>
       </c>
       <c r="C323" s="24">
-        <f t="shared" si="22"/>
-        <v>32901</v>
+        <f t="shared" si="23"/>
+        <v>32912</v>
       </c>
       <c r="F323" s="2">
+        <f t="shared" si="24"/>
+        <v>76</v>
+      </c>
+      <c r="G323" s="2">
         <v>65</v>
       </c>
       <c r="T323" s="1">
@@ -13041,10 +13132,14 @@
         <v>156</v>
       </c>
       <c r="C324" s="24">
-        <f t="shared" si="22"/>
-        <v>32922</v>
+        <f t="shared" si="23"/>
+        <v>32933</v>
       </c>
       <c r="F324" s="2">
+        <f t="shared" si="24"/>
+        <v>97</v>
+      </c>
+      <c r="G324" s="2">
         <v>86</v>
       </c>
       <c r="T324" s="1">
@@ -13059,10 +13154,14 @@
         <v>156</v>
       </c>
       <c r="C325" s="24">
-        <f t="shared" si="22"/>
-        <v>32935</v>
+        <f t="shared" si="23"/>
+        <v>32946</v>
       </c>
       <c r="F325" s="2">
+        <f t="shared" si="24"/>
+        <v>110</v>
+      </c>
+      <c r="G325" s="2">
         <v>99</v>
       </c>
       <c r="T325" s="1">
@@ -13077,10 +13176,14 @@
         <v>156</v>
       </c>
       <c r="C326" s="24">
-        <f t="shared" si="22"/>
-        <v>32948</v>
+        <f t="shared" si="23"/>
+        <v>32959</v>
       </c>
       <c r="F326" s="2">
+        <f t="shared" si="24"/>
+        <v>123</v>
+      </c>
+      <c r="G326" s="2">
         <v>112</v>
       </c>
       <c r="T326" s="1">
@@ -13095,14 +13198,21 @@
         <v>156</v>
       </c>
       <c r="C327" s="24">
-        <f t="shared" si="22"/>
-        <v>32976</v>
+        <f t="shared" si="23"/>
+        <v>32987</v>
       </c>
       <c r="D327" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F327" s="2">
+        <f t="shared" si="24"/>
+        <v>151</v>
+      </c>
+      <c r="G327" s="2">
         <v>140</v>
+      </c>
+      <c r="H327" s="1">
+        <v>11</v>
       </c>
       <c r="T327" s="1">
         <v>489.93788819875698</v>
@@ -13116,10 +13226,14 @@
         <v>157</v>
       </c>
       <c r="C328" s="24">
-        <f t="shared" si="22"/>
-        <v>32873</v>
+        <f t="shared" si="23"/>
+        <v>32884</v>
       </c>
       <c r="F328" s="2">
+        <f t="shared" si="24"/>
+        <v>48</v>
+      </c>
+      <c r="G328" s="2">
         <v>37</v>
       </c>
       <c r="T328" s="1">
@@ -13134,10 +13248,14 @@
         <v>157</v>
       </c>
       <c r="C329" s="24">
-        <f t="shared" si="22"/>
-        <v>32887</v>
+        <f t="shared" si="23"/>
+        <v>32898</v>
       </c>
       <c r="F329" s="2">
+        <f t="shared" si="24"/>
+        <v>62</v>
+      </c>
+      <c r="G329" s="2">
         <v>51</v>
       </c>
       <c r="T329" s="1">
@@ -13152,10 +13270,14 @@
         <v>157</v>
       </c>
       <c r="C330" s="24">
-        <f t="shared" si="22"/>
-        <v>32901</v>
+        <f t="shared" si="23"/>
+        <v>32912</v>
       </c>
       <c r="F330" s="2">
+        <f t="shared" si="24"/>
+        <v>76</v>
+      </c>
+      <c r="G330" s="2">
         <v>65</v>
       </c>
       <c r="T330" s="1">
@@ -13170,10 +13292,14 @@
         <v>157</v>
       </c>
       <c r="C331" s="24">
-        <f t="shared" si="22"/>
-        <v>32922</v>
+        <f t="shared" si="23"/>
+        <v>32933</v>
       </c>
       <c r="F331" s="2">
+        <f t="shared" si="24"/>
+        <v>97</v>
+      </c>
+      <c r="G331" s="2">
         <v>86</v>
       </c>
       <c r="T331" s="1">
@@ -13188,10 +13314,14 @@
         <v>157</v>
       </c>
       <c r="C332" s="24">
-        <f t="shared" si="22"/>
-        <v>32935</v>
+        <f t="shared" si="23"/>
+        <v>32946</v>
       </c>
       <c r="F332" s="2">
+        <f t="shared" si="24"/>
+        <v>110</v>
+      </c>
+      <c r="G332" s="2">
         <v>99</v>
       </c>
       <c r="T332" s="1">
@@ -13206,10 +13336,14 @@
         <v>157</v>
       </c>
       <c r="C333" s="24">
-        <f t="shared" si="22"/>
-        <v>32948</v>
+        <f t="shared" si="23"/>
+        <v>32959</v>
       </c>
       <c r="F333" s="2">
+        <f t="shared" si="24"/>
+        <v>123</v>
+      </c>
+      <c r="G333" s="2">
         <v>112</v>
       </c>
       <c r="T333" s="1">
@@ -13224,14 +13358,21 @@
         <v>157</v>
       </c>
       <c r="C334" s="24">
-        <f t="shared" si="22"/>
-        <v>32963</v>
+        <f t="shared" si="23"/>
+        <v>32974</v>
       </c>
       <c r="D334" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F334" s="2">
+        <f t="shared" si="24"/>
+        <v>138</v>
+      </c>
+      <c r="G334" s="2">
         <v>127</v>
+      </c>
+      <c r="H334" s="1">
+        <v>11</v>
       </c>
       <c r="T334" s="1">
         <v>652.90451626486902</v>
@@ -13245,10 +13386,14 @@
         <v>158</v>
       </c>
       <c r="C335" s="24">
-        <f t="shared" si="22"/>
-        <v>32873</v>
+        <f t="shared" si="23"/>
+        <v>32884</v>
       </c>
       <c r="F335" s="2">
+        <f t="shared" si="24"/>
+        <v>48</v>
+      </c>
+      <c r="G335" s="2">
         <v>37</v>
       </c>
       <c r="T335" s="1">
@@ -13263,10 +13408,14 @@
         <v>158</v>
       </c>
       <c r="C336" s="24">
-        <f t="shared" si="22"/>
-        <v>32887</v>
+        <f t="shared" si="23"/>
+        <v>32898</v>
       </c>
       <c r="F336" s="2">
+        <f t="shared" si="24"/>
+        <v>62</v>
+      </c>
+      <c r="G336" s="2">
         <v>51</v>
       </c>
       <c r="T336" s="1">
@@ -13281,10 +13430,14 @@
         <v>158</v>
       </c>
       <c r="C337" s="24">
-        <f t="shared" si="22"/>
-        <v>32901</v>
+        <f t="shared" si="23"/>
+        <v>32912</v>
       </c>
       <c r="F337" s="2">
+        <f t="shared" si="24"/>
+        <v>76</v>
+      </c>
+      <c r="G337" s="2">
         <v>65</v>
       </c>
       <c r="T337" s="1">
@@ -13299,10 +13452,14 @@
         <v>158</v>
       </c>
       <c r="C338" s="24">
-        <f t="shared" si="22"/>
-        <v>32922</v>
+        <f t="shared" si="23"/>
+        <v>32933</v>
       </c>
       <c r="F338" s="2">
+        <f t="shared" si="24"/>
+        <v>97</v>
+      </c>
+      <c r="G338" s="2">
         <v>86</v>
       </c>
       <c r="T338" s="1">
@@ -13317,10 +13474,14 @@
         <v>158</v>
       </c>
       <c r="C339" s="24">
-        <f t="shared" si="22"/>
-        <v>32935</v>
+        <f t="shared" si="23"/>
+        <v>32946</v>
       </c>
       <c r="F339" s="2">
+        <f t="shared" si="24"/>
+        <v>110</v>
+      </c>
+      <c r="G339" s="2">
         <v>99</v>
       </c>
       <c r="T339" s="1">
@@ -13335,14 +13496,21 @@
         <v>158</v>
       </c>
       <c r="C340" s="24">
-        <f t="shared" si="22"/>
-        <v>32948</v>
+        <f t="shared" si="23"/>
+        <v>32959</v>
       </c>
       <c r="D340" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F340" s="2">
+        <f t="shared" si="24"/>
+        <v>123</v>
+      </c>
+      <c r="G340" s="2">
         <v>112</v>
+      </c>
+      <c r="H340" s="1">
+        <v>11</v>
       </c>
       <c r="T340" s="1">
         <v>429.84103589851497</v>

</xml_diff>

<commit_message>
More autodoc for Gainesville
</commit_message>
<xml_diff>
--- a/Prototypes/Peanut/Observed.xlsx
+++ b/Prototypes/Peanut/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Peanut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F85F84-F919-48C8-800B-8EC42A140AD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5018B86E-FE73-4A04-8561-AF421257B965}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,6 +726,391 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Observed!$Y$276:$Y$291</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>192.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>290.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>458.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>658.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>730.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>814.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>879.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1102.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1134.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>998.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1130.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1165.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Observed!$T$276:$T$291</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>135.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>190.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>268.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>352.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>409.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>423.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>529.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E972-48E1-86E3-17FA72B59BA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="666737119"/>
+        <c:axId val="566417759"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="666737119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="566417759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="566417759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="666737119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
     <c:title>
@@ -1092,7 +1477,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1480,7 +1865,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1868,7 +2253,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2256,7 +2641,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2644,7 +3029,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3063,7 +3448,604 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>277</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>292</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03C811E4-4D4A-4083-95EE-45CBAEF679CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3248,7 +4230,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3289,7 +4271,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3636,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE028B48-E928-4E9E-80FD-208C4FFEA9B6}">
   <dimension ref="A1:AC364"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AC364"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="Y276" activeCellId="1" sqref="T276:T294 Y276:Y294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7062,7 +8044,7 @@
       </c>
       <c r="B70" s="9"/>
       <c r="C70" s="6">
-        <f t="shared" ref="C70:C103" si="3">E70+F70</f>
+        <f t="shared" ref="C70:C71" si="3">E70+F70</f>
         <v>35860</v>
       </c>
       <c r="D70" s="6"/>
@@ -20304,6 +21286,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed Kingaroy 1920 simulations (soil and Cv params)
</commit_message>
<xml_diff>
--- a/Prototypes/Peanut/Observed.xlsx
+++ b/Prototypes/Peanut/Observed.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Peanut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB12EAF-A5A1-4964-BDCD-96AE147EF65B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B776AC-AB4E-455E-B5D3-513488096D1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="12346" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="9" r:id="rId1"/>
-    <sheet name="King8485" sheetId="2" r:id="rId2"/>
-    <sheet name="Kunnunura" sheetId="3" r:id="rId3"/>
-    <sheet name="Roseworthy" sheetId="4" r:id="rId4"/>
-    <sheet name="LeafModel" sheetId="5" r:id="rId5"/>
-    <sheet name="Loxton" sheetId="6" r:id="rId6"/>
-    <sheet name="Bundy" sheetId="7" r:id="rId7"/>
-    <sheet name="Rainout" sheetId="8" r:id="rId8"/>
+    <sheet name="Kvalue" sheetId="10" r:id="rId2"/>
+    <sheet name="King8485" sheetId="2" r:id="rId3"/>
+    <sheet name="Kunnunura" sheetId="3" r:id="rId4"/>
+    <sheet name="Roseworthy" sheetId="4" r:id="rId5"/>
+    <sheet name="LeafModel" sheetId="5" r:id="rId6"/>
+    <sheet name="Loxton" sheetId="6" r:id="rId7"/>
+    <sheet name="Bundy" sheetId="7" r:id="rId8"/>
+    <sheet name="Rainout" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Treatment_Structure">#REF!</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="168">
   <si>
     <t>SimulationName</t>
   </si>
@@ -542,6 +543,12 @@
   <si>
     <t>Cover</t>
   </si>
+  <si>
+    <t>Fpar</t>
+  </si>
+  <si>
+    <t>FPAR</t>
+  </si>
 </sst>
 </file>
 
@@ -602,12 +609,34 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -616,7 +645,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -649,6 +678,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1126,6 +1157,738 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Kvalue!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fpar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Kvalue!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.1919999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0679999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6620000000000008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4820000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79599999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2240000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.5200000000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.232</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.74</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.9899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.1719999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.0600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.0020000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Kvalue!$E$2:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.28760000000000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66779999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83260000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2238</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34360000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.63280000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.68799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.31379999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.90239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24500000000000011</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.35859999999999992</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.74560000000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.68419999999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9CCD-4BAA-B1BE-ED9EEB067277}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Kvalue!$D$18:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.232</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1719999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0020000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Kvalue!$E$18:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.31379999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24500000000000011</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35859999999999992</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.74560000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.68419999999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9CCD-4BAA-B1BE-ED9EEB067277}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Kvalue!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FPAR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Kvalue!$G$2:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Kvalue!$H$2:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>5.823546641575128E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13929202357494219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25918177931828212</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.36237184837822667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45118836390597361</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.52763344725898531</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.59343034025940078</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65006225088884473</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69880578808779781</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.74075973935410844</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.77686983985157021</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.80795009137924589</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.83470111177841344</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.85772592841348638</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-9CCD-4BAA-B1BE-ED9EEB067277}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Kvalue!$H$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FPAR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Kvalue!$G$19:$G$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Kvalue!$H$19:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>7.1328306158712773E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16889571614787435</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30926566936264532</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42592773880356394</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52288608447896556</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6034685809250071</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67044103892481088</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.72610213566855442</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.77236231161618729</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.81080934201801802</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.84276283368637239</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.86931951749597491</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.891390891175042</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.90973450439021564</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-9CCD-4BAA-B1BE-ED9EEB067277}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="134003183"/>
+        <c:axId val="133996527"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="134003183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133996527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="133996527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="134003183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
     <c:title>
@@ -1492,7 +2255,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1880,7 +2643,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2268,7 +3031,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2662,7 +3425,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3050,7 +3813,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3509,7 +4272,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4068,6 +5387,47 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>594783</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>143934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>156634</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{627FB4A1-A612-4BCD-9691-2CEA3D1B4648}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -4251,7 +5611,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4292,7 +5652,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4637,16 +5997,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE028B48-E928-4E9E-80FD-208C4FFEA9B6}">
-  <dimension ref="A1:AC364"/>
+  <dimension ref="A1:AC372"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="AB57" sqref="AB57:AB58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8880" ySplit="1433" topLeftCell="H340" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A372" sqref="A372"/>
+      <selection pane="bottomRight" activeCell="M341" sqref="M341:M370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
+    <col min="1" max="1" width="33.41015625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.52734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.52734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.76171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="57.35">
@@ -20318,10 +21683,13 @@
       <c r="I341" s="2"/>
       <c r="J341" s="2"/>
       <c r="K341" s="2"/>
-      <c r="L341" s="2"/>
-      <c r="M341" s="2"/>
+      <c r="M341" s="24">
+        <v>1.1919999999999997</v>
+      </c>
       <c r="N341" s="2"/>
-      <c r="O341" s="2"/>
+      <c r="O341" s="2">
+        <v>0.28760000000000008</v>
+      </c>
       <c r="P341" s="2"/>
       <c r="Q341" s="2"/>
       <c r="R341" s="2"/>
@@ -20345,7 +21713,7 @@
       </c>
       <c r="B342" s="1"/>
       <c r="C342" s="21">
-        <f t="shared" ref="C342:C346" si="25">DATE(2019,1,10)+F342</f>
+        <f t="shared" ref="C342:C348" si="25">DATE(2019,1,10)+F342</f>
         <v>43535</v>
       </c>
       <c r="D342" s="1"/>
@@ -20358,10 +21726,13 @@
       <c r="I342" s="2"/>
       <c r="J342" s="2"/>
       <c r="K342" s="2"/>
-      <c r="L342" s="2"/>
-      <c r="M342" s="2"/>
+      <c r="M342" s="24">
+        <v>4.0679999999999996</v>
+      </c>
       <c r="N342" s="2"/>
-      <c r="O342" s="2"/>
+      <c r="O342" s="2">
+        <v>0.66779999999999995</v>
+      </c>
       <c r="P342" s="2"/>
       <c r="Q342" s="2"/>
       <c r="R342" s="2"/>
@@ -20398,10 +21769,7 @@
       <c r="I343" s="2"/>
       <c r="J343" s="2"/>
       <c r="K343" s="2"/>
-      <c r="L343" s="2"/>
-      <c r="M343" s="2"/>
       <c r="N343" s="2"/>
-      <c r="O343" s="2"/>
       <c r="P343" s="2"/>
       <c r="Q343" s="2"/>
       <c r="R343" s="2"/>
@@ -20427,37 +21795,35 @@
       </c>
       <c r="B344" s="1"/>
       <c r="C344" s="21">
-        <f t="shared" si="25"/>
-        <v>43572</v>
+        <v>43563</v>
       </c>
       <c r="D344" s="1"/>
       <c r="E344" s="1"/>
       <c r="F344" s="2">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G344" s="2"/>
       <c r="H344" s="1"/>
       <c r="I344" s="2"/>
       <c r="J344" s="2"/>
       <c r="K344" s="2"/>
-      <c r="L344" s="2"/>
-      <c r="M344" s="2"/>
+      <c r="M344" s="24">
+        <v>5.6620000000000008</v>
+      </c>
       <c r="N344" s="2"/>
-      <c r="O344" s="2"/>
+      <c r="O344" s="2">
+        <v>0.83260000000000001</v>
+      </c>
       <c r="P344" s="2"/>
       <c r="Q344" s="2"/>
       <c r="R344" s="2"/>
       <c r="S344" s="2"/>
-      <c r="T344" s="22">
-        <v>273.7</v>
-      </c>
+      <c r="T344" s="22"/>
       <c r="U344" s="2"/>
       <c r="V344" s="2"/>
       <c r="W344" s="2"/>
       <c r="X344" s="2"/>
-      <c r="Y344" s="22">
-        <v>728.2</v>
-      </c>
+      <c r="Y344" s="22"/>
       <c r="Z344" s="2"/>
       <c r="AA344" s="2"/>
       <c r="AB344" s="7"/>
@@ -20470,35 +21836,32 @@
       <c r="B345" s="1"/>
       <c r="C345" s="21">
         <f t="shared" si="25"/>
-        <v>43593</v>
+        <v>43572</v>
       </c>
       <c r="D345" s="1"/>
       <c r="E345" s="1"/>
       <c r="F345" s="2">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="G345" s="2"/>
       <c r="H345" s="1"/>
       <c r="I345" s="2"/>
       <c r="J345" s="2"/>
       <c r="K345" s="2"/>
-      <c r="L345" s="2"/>
-      <c r="M345" s="2"/>
       <c r="N345" s="2"/>
-      <c r="O345" s="2"/>
       <c r="P345" s="2"/>
       <c r="Q345" s="2"/>
       <c r="R345" s="2"/>
       <c r="S345" s="2"/>
-      <c r="T345" s="2">
-        <v>399.6</v>
+      <c r="T345" s="22">
+        <v>273.7</v>
       </c>
       <c r="U345" s="2"/>
       <c r="V345" s="2"/>
       <c r="W345" s="2"/>
       <c r="X345" s="2"/>
       <c r="Y345" s="22">
-        <v>913.9</v>
+        <v>728.2</v>
       </c>
       <c r="Z345" s="2"/>
       <c r="AA345" s="2"/>
@@ -20511,41 +21874,35 @@
       </c>
       <c r="B346" s="1"/>
       <c r="C346" s="21">
-        <f t="shared" si="25"/>
-        <v>43615</v>
-      </c>
-      <c r="D346" s="6" t="s">
-        <v>26</v>
-      </c>
+        <v>43584</v>
+      </c>
+      <c r="D346" s="1"/>
       <c r="E346" s="1"/>
       <c r="F346" s="2">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="G346" s="2"/>
       <c r="H346" s="1"/>
-      <c r="I346" s="2">
-        <v>32</v>
-      </c>
+      <c r="I346" s="2"/>
       <c r="J346" s="2"/>
       <c r="K346" s="2"/>
-      <c r="L346" s="2"/>
-      <c r="M346" s="2"/>
+      <c r="M346" s="25">
+        <v>4.4820000000000002</v>
+      </c>
       <c r="N346" s="2"/>
-      <c r="O346" s="2"/>
+      <c r="O346" s="2">
+        <v>0.80959999999999999</v>
+      </c>
       <c r="P346" s="2"/>
       <c r="Q346" s="2"/>
       <c r="R346" s="2"/>
       <c r="S346" s="2"/>
-      <c r="T346" s="22">
-        <v>412.7</v>
-      </c>
+      <c r="T346" s="22"/>
       <c r="U346" s="2"/>
       <c r="V346" s="2"/>
       <c r="W346" s="2"/>
       <c r="X346" s="2"/>
-      <c r="Y346" s="22">
-        <v>831.6</v>
-      </c>
+      <c r="Y346" s="22"/>
       <c r="Z346" s="2"/>
       <c r="AA346" s="2"/>
       <c r="AB346" s="7"/>
@@ -20553,24 +21910,23 @@
     </row>
     <row r="347" spans="1:29">
       <c r="A347" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B347" s="1"/>
       <c r="C347" s="21">
-        <f>DATE(2019,1,10)+F347</f>
-        <v>43514</v>
+        <f t="shared" si="25"/>
+        <v>43593</v>
       </c>
       <c r="D347" s="1"/>
       <c r="E347" s="1"/>
       <c r="F347" s="2">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="G347" s="2"/>
       <c r="H347" s="1"/>
       <c r="I347" s="2"/>
       <c r="J347" s="2"/>
       <c r="K347" s="2"/>
-      <c r="L347" s="2"/>
       <c r="M347" s="2"/>
       <c r="N347" s="2"/>
       <c r="O347" s="2"/>
@@ -20578,13 +21934,15 @@
       <c r="Q347" s="2"/>
       <c r="R347" s="2"/>
       <c r="S347" s="2"/>
-      <c r="T347" s="2"/>
+      <c r="T347" s="2">
+        <v>399.6</v>
+      </c>
       <c r="U347" s="2"/>
       <c r="V347" s="2"/>
       <c r="W347" s="2"/>
       <c r="X347" s="2"/>
       <c r="Y347" s="22">
-        <v>103.5</v>
+        <v>913.9</v>
       </c>
       <c r="Z347" s="2"/>
       <c r="AA347" s="2"/>
@@ -20593,24 +21951,27 @@
     </row>
     <row r="348" spans="1:29">
       <c r="A348" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B348" s="1"/>
       <c r="C348" s="21">
-        <f t="shared" ref="C348:C352" si="26">DATE(2019,1,10)+F348</f>
-        <v>43535</v>
-      </c>
-      <c r="D348" s="1"/>
+        <f t="shared" si="25"/>
+        <v>43615</v>
+      </c>
+      <c r="D348" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="E348" s="1"/>
       <c r="F348" s="2">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="G348" s="2"/>
       <c r="H348" s="1"/>
-      <c r="I348" s="2"/>
+      <c r="I348" s="2">
+        <v>32</v>
+      </c>
       <c r="J348" s="2"/>
       <c r="K348" s="2"/>
-      <c r="L348" s="2"/>
       <c r="M348" s="2"/>
       <c r="N348" s="2"/>
       <c r="O348" s="2"/>
@@ -20618,13 +21979,15 @@
       <c r="Q348" s="2"/>
       <c r="R348" s="2"/>
       <c r="S348" s="2"/>
-      <c r="T348" s="2"/>
+      <c r="T348" s="22">
+        <v>412.7</v>
+      </c>
       <c r="U348" s="2"/>
       <c r="V348" s="2"/>
       <c r="W348" s="2"/>
       <c r="X348" s="2"/>
       <c r="Y348" s="22">
-        <v>233.6</v>
+        <v>831.6</v>
       </c>
       <c r="Z348" s="2"/>
       <c r="AA348" s="2"/>
@@ -20637,36 +22000,37 @@
       </c>
       <c r="B349" s="1"/>
       <c r="C349" s="21">
-        <f t="shared" si="26"/>
-        <v>43557</v>
+        <f>DATE(2019,1,10)+F349</f>
+        <v>43514</v>
       </c>
       <c r="D349" s="1"/>
       <c r="E349" s="1"/>
       <c r="F349" s="2">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="G349" s="2"/>
       <c r="H349" s="1"/>
       <c r="I349" s="2"/>
       <c r="J349" s="2"/>
       <c r="K349" s="2"/>
-      <c r="L349" s="2"/>
-      <c r="M349" s="2"/>
+      <c r="M349" s="24">
+        <v>0.79599999999999993</v>
+      </c>
       <c r="N349" s="2"/>
-      <c r="O349" s="2"/>
+      <c r="O349" s="2">
+        <v>0.2238</v>
+      </c>
       <c r="P349" s="2"/>
       <c r="Q349" s="2"/>
       <c r="R349" s="2"/>
       <c r="S349" s="2"/>
-      <c r="T349" s="22">
-        <v>54.9</v>
-      </c>
+      <c r="T349" s="2"/>
       <c r="U349" s="2"/>
       <c r="V349" s="2"/>
       <c r="W349" s="2"/>
       <c r="X349" s="2"/>
       <c r="Y349" s="22">
-        <v>372.6</v>
+        <v>103.5</v>
       </c>
       <c r="Z349" s="2"/>
       <c r="AA349" s="2"/>
@@ -20679,36 +22043,37 @@
       </c>
       <c r="B350" s="1"/>
       <c r="C350" s="21">
-        <f t="shared" si="26"/>
-        <v>43572</v>
+        <f t="shared" ref="C350:C356" si="26">DATE(2019,1,10)+F350</f>
+        <v>43535</v>
       </c>
       <c r="D350" s="1"/>
       <c r="E350" s="1"/>
       <c r="F350" s="2">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="G350" s="2"/>
       <c r="H350" s="1"/>
       <c r="I350" s="2"/>
       <c r="J350" s="2"/>
       <c r="K350" s="2"/>
-      <c r="L350" s="2"/>
-      <c r="M350" s="2"/>
+      <c r="M350" s="24">
+        <v>1.2240000000000002</v>
+      </c>
       <c r="N350" s="2"/>
-      <c r="O350" s="2"/>
+      <c r="O350" s="2">
+        <v>0.34360000000000002</v>
+      </c>
       <c r="P350" s="2"/>
       <c r="Q350" s="2"/>
       <c r="R350" s="2"/>
       <c r="S350" s="2"/>
-      <c r="T350" s="22">
-        <v>136.1</v>
-      </c>
+      <c r="T350" s="2"/>
       <c r="U350" s="2"/>
       <c r="V350" s="2"/>
       <c r="W350" s="2"/>
       <c r="X350" s="2"/>
       <c r="Y350" s="22">
-        <v>517.9</v>
+        <v>233.6</v>
       </c>
       <c r="Z350" s="2"/>
       <c r="AA350" s="2"/>
@@ -20722,35 +22087,32 @@
       <c r="B351" s="1"/>
       <c r="C351" s="21">
         <f t="shared" si="26"/>
-        <v>43593</v>
+        <v>43557</v>
       </c>
       <c r="D351" s="1"/>
       <c r="E351" s="1"/>
       <c r="F351" s="2">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="G351" s="2"/>
       <c r="H351" s="1"/>
       <c r="I351" s="2"/>
       <c r="J351" s="2"/>
       <c r="K351" s="2"/>
-      <c r="L351" s="2"/>
-      <c r="M351" s="2"/>
       <c r="N351" s="2"/>
-      <c r="O351" s="2"/>
       <c r="P351" s="2"/>
       <c r="Q351" s="2"/>
       <c r="R351" s="2"/>
       <c r="S351" s="2"/>
       <c r="T351" s="22">
-        <v>260.10000000000002</v>
+        <v>54.9</v>
       </c>
       <c r="U351" s="2"/>
       <c r="V351" s="2"/>
       <c r="W351" s="2"/>
       <c r="X351" s="2"/>
       <c r="Y351" s="22">
-        <v>656.4</v>
+        <v>372.6</v>
       </c>
       <c r="Z351" s="2"/>
       <c r="AA351" s="2"/>
@@ -20763,41 +22125,35 @@
       </c>
       <c r="B352" s="1"/>
       <c r="C352" s="21">
-        <f t="shared" si="26"/>
-        <v>43615</v>
-      </c>
-      <c r="D352" s="6" t="s">
-        <v>26</v>
-      </c>
+        <v>43563</v>
+      </c>
+      <c r="D352" s="1"/>
       <c r="E352" s="1"/>
       <c r="F352" s="2">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="G352" s="2"/>
       <c r="H352" s="1"/>
-      <c r="I352" s="2">
-        <v>32</v>
-      </c>
+      <c r="I352" s="2"/>
       <c r="J352" s="2"/>
       <c r="K352" s="2"/>
-      <c r="L352" s="2"/>
-      <c r="M352" s="2"/>
+      <c r="M352" s="24">
+        <v>3.6719999999999997</v>
+      </c>
       <c r="N352" s="2"/>
-      <c r="O352" s="2"/>
+      <c r="O352" s="2">
+        <v>0.63280000000000003</v>
+      </c>
       <c r="P352" s="2"/>
       <c r="Q352" s="2"/>
       <c r="R352" s="2"/>
       <c r="S352" s="2"/>
-      <c r="T352" s="22">
-        <v>323</v>
-      </c>
+      <c r="T352" s="22"/>
       <c r="U352" s="2"/>
       <c r="V352" s="2"/>
       <c r="W352" s="2"/>
       <c r="X352" s="2"/>
-      <c r="Y352" s="22">
-        <v>707.5</v>
-      </c>
+      <c r="Y352" s="22"/>
       <c r="Z352" s="2"/>
       <c r="AA352" s="2"/>
       <c r="AB352" s="7"/>
@@ -20805,38 +22161,37 @@
     </row>
     <row r="353" spans="1:29">
       <c r="A353" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B353" s="1"/>
       <c r="C353" s="21">
-        <f>DATE(2019,1,10)+F353</f>
-        <v>43514</v>
+        <f t="shared" si="26"/>
+        <v>43572</v>
       </c>
       <c r="D353" s="1"/>
       <c r="E353" s="1"/>
       <c r="F353" s="2">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="G353" s="2"/>
       <c r="H353" s="1"/>
       <c r="I353" s="2"/>
       <c r="J353" s="2"/>
       <c r="K353" s="2"/>
-      <c r="L353" s="2"/>
-      <c r="M353" s="2"/>
       <c r="N353" s="2"/>
-      <c r="O353" s="2"/>
       <c r="P353" s="2"/>
       <c r="Q353" s="2"/>
       <c r="R353" s="2"/>
       <c r="S353" s="2"/>
-      <c r="T353" s="2"/>
+      <c r="T353" s="22">
+        <v>136.1</v>
+      </c>
       <c r="U353" s="2"/>
       <c r="V353" s="2"/>
       <c r="W353" s="2"/>
       <c r="X353" s="2"/>
       <c r="Y353" s="22">
-        <v>89.5</v>
+        <v>517.9</v>
       </c>
       <c r="Z353" s="2"/>
       <c r="AA353" s="2"/>
@@ -20845,39 +22200,39 @@
     </row>
     <row r="354" spans="1:29">
       <c r="A354" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B354" s="1"/>
       <c r="C354" s="21">
-        <f t="shared" ref="C354:C358" si="27">DATE(2019,1,10)+F354</f>
-        <v>43535</v>
+        <v>43584</v>
       </c>
       <c r="D354" s="1"/>
       <c r="E354" s="1"/>
       <c r="F354" s="2">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="G354" s="2"/>
       <c r="H354" s="1"/>
       <c r="I354" s="2"/>
       <c r="J354" s="2"/>
       <c r="K354" s="2"/>
-      <c r="L354" s="2"/>
-      <c r="M354" s="2"/>
+      <c r="M354" s="25">
+        <v>3.5200000000000005</v>
+      </c>
       <c r="N354" s="2"/>
-      <c r="O354" s="2"/>
+      <c r="O354" s="2">
+        <v>0.68799999999999994</v>
+      </c>
       <c r="P354" s="2"/>
       <c r="Q354" s="2"/>
       <c r="R354" s="2"/>
       <c r="S354" s="2"/>
-      <c r="T354" s="2"/>
+      <c r="T354" s="22"/>
       <c r="U354" s="2"/>
       <c r="V354" s="2"/>
       <c r="W354" s="2"/>
       <c r="X354" s="2"/>
-      <c r="Y354" s="22">
-        <v>340.4</v>
-      </c>
+      <c r="Y354" s="22"/>
       <c r="Z354" s="2"/>
       <c r="AA354" s="2"/>
       <c r="AB354" s="7"/>
@@ -20885,24 +22240,23 @@
     </row>
     <row r="355" spans="1:29">
       <c r="A355" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B355" s="1"/>
       <c r="C355" s="21">
-        <f t="shared" si="27"/>
-        <v>43557</v>
+        <f t="shared" si="26"/>
+        <v>43593</v>
       </c>
       <c r="D355" s="1"/>
       <c r="E355" s="1"/>
       <c r="F355" s="2">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="G355" s="2"/>
       <c r="H355" s="1"/>
       <c r="I355" s="2"/>
       <c r="J355" s="2"/>
       <c r="K355" s="2"/>
-      <c r="L355" s="2"/>
       <c r="M355" s="2"/>
       <c r="N355" s="2"/>
       <c r="O355" s="2"/>
@@ -20911,14 +22265,14 @@
       <c r="R355" s="2"/>
       <c r="S355" s="2"/>
       <c r="T355" s="22">
-        <v>129.5</v>
+        <v>260.10000000000002</v>
       </c>
       <c r="U355" s="2"/>
       <c r="V355" s="2"/>
       <c r="W355" s="2"/>
       <c r="X355" s="2"/>
       <c r="Y355" s="22">
-        <v>606.4</v>
+        <v>656.4</v>
       </c>
       <c r="Z355" s="2"/>
       <c r="AA355" s="2"/>
@@ -20927,24 +22281,27 @@
     </row>
     <row r="356" spans="1:29">
       <c r="A356" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B356" s="1"/>
       <c r="C356" s="21">
-        <f t="shared" si="27"/>
-        <v>43572</v>
-      </c>
-      <c r="D356" s="1"/>
+        <f t="shared" si="26"/>
+        <v>43615</v>
+      </c>
+      <c r="D356" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="E356" s="1"/>
       <c r="F356" s="2">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="G356" s="2"/>
       <c r="H356" s="1"/>
-      <c r="I356" s="2"/>
+      <c r="I356" s="2">
+        <v>32</v>
+      </c>
       <c r="J356" s="2"/>
       <c r="K356" s="2"/>
-      <c r="L356" s="2"/>
       <c r="M356" s="2"/>
       <c r="N356" s="2"/>
       <c r="O356" s="2"/>
@@ -20953,14 +22310,14 @@
       <c r="R356" s="2"/>
       <c r="S356" s="2"/>
       <c r="T356" s="22">
-        <v>236.1</v>
+        <v>323</v>
       </c>
       <c r="U356" s="2"/>
       <c r="V356" s="2"/>
       <c r="W356" s="2"/>
       <c r="X356" s="2"/>
       <c r="Y356" s="22">
-        <v>721.5</v>
+        <v>707.5</v>
       </c>
       <c r="Z356" s="2"/>
       <c r="AA356" s="2"/>
@@ -20973,36 +22330,37 @@
       </c>
       <c r="B357" s="1"/>
       <c r="C357" s="21">
-        <f t="shared" si="27"/>
-        <v>43593</v>
+        <f>DATE(2019,1,10)+F357</f>
+        <v>43514</v>
       </c>
       <c r="D357" s="1"/>
       <c r="E357" s="1"/>
       <c r="F357" s="2">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="G357" s="2"/>
       <c r="H357" s="1"/>
       <c r="I357" s="2"/>
       <c r="J357" s="2"/>
       <c r="K357" s="2"/>
-      <c r="L357" s="2"/>
-      <c r="M357" s="2"/>
+      <c r="M357" s="24">
+        <v>1.232</v>
+      </c>
       <c r="N357" s="2"/>
-      <c r="O357" s="2"/>
+      <c r="O357" s="2">
+        <v>0.31379999999999997</v>
+      </c>
       <c r="P357" s="2"/>
       <c r="Q357" s="2"/>
       <c r="R357" s="2"/>
       <c r="S357" s="2"/>
-      <c r="T357" s="22">
-        <v>434.2</v>
-      </c>
+      <c r="T357" s="2"/>
       <c r="U357" s="2"/>
       <c r="V357" s="2"/>
       <c r="W357" s="2"/>
       <c r="X357" s="2"/>
       <c r="Y357" s="22">
-        <v>976</v>
+        <v>89.5</v>
       </c>
       <c r="Z357" s="2"/>
       <c r="AA357" s="2"/>
@@ -21015,40 +22373,37 @@
       </c>
       <c r="B358" s="1"/>
       <c r="C358" s="21">
-        <f t="shared" si="27"/>
-        <v>43615</v>
-      </c>
-      <c r="D358" s="6" t="s">
-        <v>26</v>
-      </c>
+        <f t="shared" ref="C358:C364" si="27">DATE(2019,1,10)+F358</f>
+        <v>43535</v>
+      </c>
+      <c r="D358" s="1"/>
       <c r="E358" s="1"/>
       <c r="F358" s="2">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="G358" s="2"/>
       <c r="H358" s="1"/>
-      <c r="I358" s="2">
-        <v>32</v>
-      </c>
+      <c r="I358" s="2"/>
       <c r="J358" s="2"/>
       <c r="K358" s="2"/>
-      <c r="L358" s="2"/>
-      <c r="M358" s="2"/>
+      <c r="M358" s="24">
+        <v>3.1719999999999997</v>
+      </c>
       <c r="N358" s="2"/>
-      <c r="O358" s="2"/>
+      <c r="O358" s="2">
+        <v>0.66200000000000003</v>
+      </c>
       <c r="P358" s="2"/>
       <c r="Q358" s="2"/>
       <c r="R358" s="2"/>
       <c r="S358" s="2"/>
-      <c r="T358" s="22">
-        <v>451.8</v>
-      </c>
+      <c r="T358" s="2"/>
       <c r="U358" s="2"/>
       <c r="V358" s="2"/>
       <c r="W358" s="2"/>
       <c r="X358" s="2"/>
       <c r="Y358" s="22">
-        <v>959.6</v>
+        <v>340.4</v>
       </c>
       <c r="Z358" s="2"/>
       <c r="AA358" s="2"/>
@@ -21057,38 +22412,37 @@
     </row>
     <row r="359" spans="1:29">
       <c r="A359" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B359" s="1"/>
       <c r="C359" s="21">
-        <f>DATE(2019,1,10)+F359</f>
-        <v>43514</v>
+        <f t="shared" si="27"/>
+        <v>43557</v>
       </c>
       <c r="D359" s="1"/>
       <c r="E359" s="1"/>
       <c r="F359" s="2">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="G359" s="2"/>
       <c r="H359" s="1"/>
       <c r="I359" s="2"/>
       <c r="J359" s="2"/>
       <c r="K359" s="2"/>
-      <c r="L359" s="2"/>
-      <c r="M359" s="2"/>
       <c r="N359" s="2"/>
-      <c r="O359" s="2"/>
       <c r="P359" s="2"/>
       <c r="Q359" s="2"/>
       <c r="R359" s="2"/>
       <c r="S359" s="2"/>
-      <c r="T359" s="2"/>
+      <c r="T359" s="22">
+        <v>129.5</v>
+      </c>
       <c r="U359" s="2"/>
       <c r="V359" s="2"/>
       <c r="W359" s="2"/>
       <c r="X359" s="2"/>
       <c r="Y359" s="22">
-        <v>87.7</v>
+        <v>606.4</v>
       </c>
       <c r="Z359" s="2"/>
       <c r="AA359" s="2"/>
@@ -21097,39 +22451,39 @@
     </row>
     <row r="360" spans="1:29">
       <c r="A360" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B360" s="1"/>
       <c r="C360" s="21">
-        <f t="shared" ref="C360:C364" si="28">DATE(2019,1,10)+F360</f>
-        <v>43535</v>
+        <v>43563</v>
       </c>
       <c r="D360" s="1"/>
       <c r="E360" s="1"/>
       <c r="F360" s="2">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="G360" s="2"/>
       <c r="H360" s="1"/>
       <c r="I360" s="2"/>
       <c r="J360" s="2"/>
       <c r="K360" s="2"/>
-      <c r="L360" s="2"/>
-      <c r="M360" s="2"/>
+      <c r="M360" s="24">
+        <v>5.74</v>
+      </c>
       <c r="N360" s="2"/>
-      <c r="O360" s="2"/>
+      <c r="O360" s="2">
+        <v>0.90239999999999998</v>
+      </c>
       <c r="P360" s="2"/>
       <c r="Q360" s="2"/>
       <c r="R360" s="2"/>
       <c r="S360" s="2"/>
-      <c r="T360" s="2"/>
+      <c r="T360" s="22"/>
       <c r="U360" s="2"/>
       <c r="V360" s="2"/>
       <c r="W360" s="2"/>
       <c r="X360" s="2"/>
-      <c r="Y360" s="22">
-        <v>201</v>
-      </c>
+      <c r="Y360" s="22"/>
       <c r="Z360" s="2"/>
       <c r="AA360" s="2"/>
       <c r="AB360" s="7"/>
@@ -21137,40 +22491,37 @@
     </row>
     <row r="361" spans="1:29">
       <c r="A361" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B361" s="1"/>
       <c r="C361" s="21">
-        <f t="shared" si="28"/>
-        <v>43557</v>
+        <f t="shared" si="27"/>
+        <v>43572</v>
       </c>
       <c r="D361" s="1"/>
       <c r="E361" s="1"/>
       <c r="F361" s="2">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="G361" s="2"/>
       <c r="H361" s="1"/>
       <c r="I361" s="2"/>
       <c r="J361" s="2"/>
       <c r="K361" s="2"/>
-      <c r="L361" s="2"/>
-      <c r="M361" s="2"/>
       <c r="N361" s="2"/>
-      <c r="O361" s="2"/>
       <c r="P361" s="2"/>
       <c r="Q361" s="2"/>
       <c r="R361" s="2"/>
       <c r="S361" s="2"/>
       <c r="T361" s="22">
-        <v>50</v>
+        <v>236.1</v>
       </c>
       <c r="U361" s="2"/>
       <c r="V361" s="2"/>
       <c r="W361" s="2"/>
       <c r="X361" s="2"/>
       <c r="Y361" s="22">
-        <v>367.2</v>
+        <v>721.5</v>
       </c>
       <c r="Z361" s="2"/>
       <c r="AA361" s="2"/>
@@ -21179,41 +22530,39 @@
     </row>
     <row r="362" spans="1:29">
       <c r="A362" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B362" s="1"/>
       <c r="C362" s="21">
-        <f t="shared" si="28"/>
-        <v>43572</v>
+        <v>43584</v>
       </c>
       <c r="D362" s="1"/>
       <c r="E362" s="1"/>
       <c r="F362" s="2">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="G362" s="2"/>
       <c r="H362" s="1"/>
       <c r="I362" s="2"/>
       <c r="J362" s="2"/>
       <c r="K362" s="2"/>
-      <c r="L362" s="2"/>
-      <c r="M362" s="2"/>
+      <c r="M362" s="25">
+        <v>3.9899999999999998</v>
+      </c>
       <c r="N362" s="2"/>
-      <c r="O362" s="2"/>
+      <c r="O362" s="2">
+        <v>0.81</v>
+      </c>
       <c r="P362" s="2"/>
       <c r="Q362" s="2"/>
       <c r="R362" s="2"/>
       <c r="S362" s="2"/>
-      <c r="T362" s="22">
-        <v>136.4</v>
-      </c>
+      <c r="T362" s="22"/>
       <c r="U362" s="2"/>
       <c r="V362" s="2"/>
       <c r="W362" s="2"/>
       <c r="X362" s="2"/>
-      <c r="Y362" s="22">
-        <v>489.6</v>
-      </c>
+      <c r="Y362" s="22"/>
       <c r="Z362" s="2"/>
       <c r="AA362" s="2"/>
       <c r="AB362" s="7"/>
@@ -21221,11 +22570,11 @@
     </row>
     <row r="363" spans="1:29">
       <c r="A363" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B363" s="1"/>
       <c r="C363" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>43593</v>
       </c>
       <c r="D363" s="1"/>
@@ -21238,7 +22587,6 @@
       <c r="I363" s="2"/>
       <c r="J363" s="2"/>
       <c r="K363" s="2"/>
-      <c r="L363" s="2"/>
       <c r="M363" s="2"/>
       <c r="N363" s="2"/>
       <c r="O363" s="2"/>
@@ -21247,14 +22595,14 @@
       <c r="R363" s="2"/>
       <c r="S363" s="2"/>
       <c r="T363" s="22">
-        <v>283</v>
+        <v>434.2</v>
       </c>
       <c r="U363" s="2"/>
       <c r="V363" s="2"/>
       <c r="W363" s="2"/>
       <c r="X363" s="2"/>
       <c r="Y363" s="22">
-        <v>686</v>
+        <v>976</v>
       </c>
       <c r="Z363" s="2"/>
       <c r="AA363" s="2"/>
@@ -21263,11 +22611,11 @@
     </row>
     <row r="364" spans="1:29">
       <c r="A364" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B364" s="1"/>
       <c r="C364" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>43615</v>
       </c>
       <c r="D364" s="6" t="s">
@@ -21284,7 +22632,6 @@
       </c>
       <c r="J364" s="2"/>
       <c r="K364" s="2"/>
-      <c r="L364" s="2"/>
       <c r="M364" s="2"/>
       <c r="N364" s="2"/>
       <c r="O364" s="2"/>
@@ -21293,19 +22640,351 @@
       <c r="R364" s="2"/>
       <c r="S364" s="2"/>
       <c r="T364" s="22">
-        <v>281.60000000000002</v>
+        <v>451.8</v>
       </c>
       <c r="U364" s="2"/>
       <c r="V364" s="2"/>
       <c r="W364" s="2"/>
       <c r="X364" s="2"/>
       <c r="Y364" s="22">
-        <v>640.79999999999995</v>
+        <v>959.6</v>
       </c>
       <c r="Z364" s="2"/>
       <c r="AA364" s="2"/>
       <c r="AB364" s="7"/>
       <c r="AC364" s="7"/>
+    </row>
+    <row r="365" spans="1:29">
+      <c r="A365" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B365" s="1"/>
+      <c r="C365" s="21">
+        <f>DATE(2019,1,10)+F365</f>
+        <v>43514</v>
+      </c>
+      <c r="D365" s="1"/>
+      <c r="E365" s="1"/>
+      <c r="F365" s="2">
+        <v>39</v>
+      </c>
+      <c r="G365" s="2"/>
+      <c r="H365" s="1"/>
+      <c r="I365" s="2"/>
+      <c r="J365" s="2"/>
+      <c r="K365" s="2"/>
+      <c r="M365" s="24">
+        <v>0.85</v>
+      </c>
+      <c r="N365" s="2"/>
+      <c r="O365" s="2">
+        <v>0.24500000000000011</v>
+      </c>
+      <c r="P365" s="2"/>
+      <c r="Q365" s="2"/>
+      <c r="R365" s="2"/>
+      <c r="S365" s="2"/>
+      <c r="T365" s="2"/>
+      <c r="U365" s="2"/>
+      <c r="V365" s="2"/>
+      <c r="W365" s="2"/>
+      <c r="X365" s="2"/>
+      <c r="Y365" s="22">
+        <v>87.7</v>
+      </c>
+      <c r="Z365" s="2"/>
+      <c r="AA365" s="2"/>
+      <c r="AB365" s="7"/>
+      <c r="AC365" s="7"/>
+    </row>
+    <row r="366" spans="1:29">
+      <c r="A366" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B366" s="1"/>
+      <c r="C366" s="21">
+        <f t="shared" ref="C366:C372" si="28">DATE(2019,1,10)+F366</f>
+        <v>43535</v>
+      </c>
+      <c r="D366" s="1"/>
+      <c r="E366" s="1"/>
+      <c r="F366" s="2">
+        <v>60</v>
+      </c>
+      <c r="G366" s="2"/>
+      <c r="H366" s="1"/>
+      <c r="I366" s="2"/>
+      <c r="J366" s="2"/>
+      <c r="K366" s="2"/>
+      <c r="M366" s="24">
+        <v>1.1719999999999999</v>
+      </c>
+      <c r="N366" s="2"/>
+      <c r="O366" s="2">
+        <v>0.35859999999999992</v>
+      </c>
+      <c r="P366" s="2"/>
+      <c r="Q366" s="2"/>
+      <c r="R366" s="2"/>
+      <c r="S366" s="2"/>
+      <c r="T366" s="2"/>
+      <c r="U366" s="2"/>
+      <c r="V366" s="2"/>
+      <c r="W366" s="2"/>
+      <c r="X366" s="2"/>
+      <c r="Y366" s="22">
+        <v>201</v>
+      </c>
+      <c r="Z366" s="2"/>
+      <c r="AA366" s="2"/>
+      <c r="AB366" s="7"/>
+      <c r="AC366" s="7"/>
+    </row>
+    <row r="367" spans="1:29">
+      <c r="A367" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B367" s="1"/>
+      <c r="C367" s="21">
+        <f t="shared" si="28"/>
+        <v>43557</v>
+      </c>
+      <c r="D367" s="1"/>
+      <c r="E367" s="1"/>
+      <c r="F367" s="2">
+        <v>82</v>
+      </c>
+      <c r="G367" s="2"/>
+      <c r="H367" s="1"/>
+      <c r="I367" s="2"/>
+      <c r="J367" s="2"/>
+      <c r="K367" s="2"/>
+      <c r="N367" s="2"/>
+      <c r="P367" s="2"/>
+      <c r="Q367" s="2"/>
+      <c r="R367" s="2"/>
+      <c r="S367" s="2"/>
+      <c r="T367" s="22">
+        <v>50</v>
+      </c>
+      <c r="U367" s="2"/>
+      <c r="V367" s="2"/>
+      <c r="W367" s="2"/>
+      <c r="X367" s="2"/>
+      <c r="Y367" s="22">
+        <v>367.2</v>
+      </c>
+      <c r="Z367" s="2"/>
+      <c r="AA367" s="2"/>
+      <c r="AB367" s="7"/>
+      <c r="AC367" s="7"/>
+    </row>
+    <row r="368" spans="1:29">
+      <c r="A368" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B368" s="1"/>
+      <c r="C368" s="21">
+        <v>43563</v>
+      </c>
+      <c r="D368" s="1"/>
+      <c r="E368" s="1"/>
+      <c r="F368" s="2">
+        <v>88</v>
+      </c>
+      <c r="G368" s="2"/>
+      <c r="H368" s="1"/>
+      <c r="I368" s="2"/>
+      <c r="J368" s="2"/>
+      <c r="K368" s="2"/>
+      <c r="M368" s="24">
+        <v>4.0600000000000005</v>
+      </c>
+      <c r="N368" s="2"/>
+      <c r="O368" s="2">
+        <v>0.74560000000000004</v>
+      </c>
+      <c r="P368" s="2"/>
+      <c r="Q368" s="2"/>
+      <c r="R368" s="2"/>
+      <c r="S368" s="2"/>
+      <c r="T368" s="22"/>
+      <c r="U368" s="2"/>
+      <c r="V368" s="2"/>
+      <c r="W368" s="2"/>
+      <c r="X368" s="2"/>
+      <c r="Y368" s="22"/>
+      <c r="Z368" s="2"/>
+      <c r="AA368" s="2"/>
+      <c r="AB368" s="7"/>
+      <c r="AC368" s="7"/>
+    </row>
+    <row r="369" spans="1:29">
+      <c r="A369" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B369" s="1"/>
+      <c r="C369" s="21">
+        <f t="shared" si="28"/>
+        <v>43572</v>
+      </c>
+      <c r="D369" s="1"/>
+      <c r="E369" s="1"/>
+      <c r="F369" s="2">
+        <v>97</v>
+      </c>
+      <c r="G369" s="2"/>
+      <c r="H369" s="1"/>
+      <c r="I369" s="2"/>
+      <c r="J369" s="2"/>
+      <c r="K369" s="2"/>
+      <c r="N369" s="2"/>
+      <c r="P369" s="2"/>
+      <c r="Q369" s="2"/>
+      <c r="R369" s="2"/>
+      <c r="S369" s="2"/>
+      <c r="T369" s="22">
+        <v>136.4</v>
+      </c>
+      <c r="U369" s="2"/>
+      <c r="V369" s="2"/>
+      <c r="W369" s="2"/>
+      <c r="X369" s="2"/>
+      <c r="Y369" s="22">
+        <v>489.6</v>
+      </c>
+      <c r="Z369" s="2"/>
+      <c r="AA369" s="2"/>
+      <c r="AB369" s="7"/>
+      <c r="AC369" s="7"/>
+    </row>
+    <row r="370" spans="1:29">
+      <c r="A370" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B370" s="1"/>
+      <c r="C370" s="21">
+        <v>43584</v>
+      </c>
+      <c r="D370" s="1"/>
+      <c r="E370" s="1"/>
+      <c r="F370" s="2">
+        <v>109</v>
+      </c>
+      <c r="G370" s="2"/>
+      <c r="H370" s="1"/>
+      <c r="I370" s="2"/>
+      <c r="J370" s="2"/>
+      <c r="K370" s="2"/>
+      <c r="M370" s="25">
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="N370" s="2"/>
+      <c r="O370" s="2">
+        <v>0.68419999999999992</v>
+      </c>
+      <c r="P370" s="2"/>
+      <c r="Q370" s="2"/>
+      <c r="R370" s="2"/>
+      <c r="S370" s="2"/>
+      <c r="T370" s="22"/>
+      <c r="U370" s="2"/>
+      <c r="V370" s="2"/>
+      <c r="W370" s="2"/>
+      <c r="X370" s="2"/>
+      <c r="Y370" s="22"/>
+      <c r="Z370" s="2"/>
+      <c r="AA370" s="2"/>
+      <c r="AB370" s="7"/>
+      <c r="AC370" s="7"/>
+    </row>
+    <row r="371" spans="1:29">
+      <c r="A371" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B371" s="1"/>
+      <c r="C371" s="21">
+        <f t="shared" si="28"/>
+        <v>43593</v>
+      </c>
+      <c r="D371" s="1"/>
+      <c r="E371" s="1"/>
+      <c r="F371" s="2">
+        <v>118</v>
+      </c>
+      <c r="G371" s="2"/>
+      <c r="H371" s="1"/>
+      <c r="I371" s="2"/>
+      <c r="J371" s="2"/>
+      <c r="K371" s="2"/>
+      <c r="L371" s="2"/>
+      <c r="M371" s="2"/>
+      <c r="N371" s="2"/>
+      <c r="O371" s="2"/>
+      <c r="P371" s="2"/>
+      <c r="Q371" s="2"/>
+      <c r="R371" s="2"/>
+      <c r="S371" s="2"/>
+      <c r="T371" s="22">
+        <v>283</v>
+      </c>
+      <c r="U371" s="2"/>
+      <c r="V371" s="2"/>
+      <c r="W371" s="2"/>
+      <c r="X371" s="2"/>
+      <c r="Y371" s="22">
+        <v>686</v>
+      </c>
+      <c r="Z371" s="2"/>
+      <c r="AA371" s="2"/>
+      <c r="AB371" s="7"/>
+      <c r="AC371" s="7"/>
+    </row>
+    <row r="372" spans="1:29">
+      <c r="A372" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B372" s="1"/>
+      <c r="C372" s="21">
+        <f t="shared" si="28"/>
+        <v>43615</v>
+      </c>
+      <c r="D372" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E372" s="1"/>
+      <c r="F372" s="2">
+        <v>140</v>
+      </c>
+      <c r="G372" s="2"/>
+      <c r="H372" s="1"/>
+      <c r="I372" s="2">
+        <v>32</v>
+      </c>
+      <c r="J372" s="2"/>
+      <c r="K372" s="2"/>
+      <c r="L372" s="2"/>
+      <c r="M372" s="2"/>
+      <c r="N372" s="2"/>
+      <c r="O372" s="2"/>
+      <c r="P372" s="2"/>
+      <c r="Q372" s="2"/>
+      <c r="R372" s="2"/>
+      <c r="S372" s="2"/>
+      <c r="T372" s="22">
+        <v>281.60000000000002</v>
+      </c>
+      <c r="U372" s="2"/>
+      <c r="V372" s="2"/>
+      <c r="W372" s="2"/>
+      <c r="X372" s="2"/>
+      <c r="Y372" s="22">
+        <v>640.79999999999995</v>
+      </c>
+      <c r="Z372" s="2"/>
+      <c r="AA372" s="2"/>
+      <c r="AB372" s="7"/>
+      <c r="AC372" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21315,6 +22994,438 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E255DA-0239-41A0-B7F2-1E7C5BB2D43C}">
+  <dimension ref="D1:I32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35"/>
+  <sheetData>
+    <row r="1" spans="4:9">
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="4:9">
+      <c r="D2" s="24">
+        <v>1.1919999999999997</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.28760000000000008</v>
+      </c>
+      <c r="G2">
+        <v>0.2</v>
+      </c>
+      <c r="H2">
+        <f>1-EXP(-$I$2*G2)</f>
+        <v>5.823546641575128E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="4:9">
+      <c r="D3" s="24">
+        <v>4.0679999999999996</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.66779999999999995</v>
+      </c>
+      <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H15" si="0">1-EXP(-$I$2*G3)</f>
+        <v>0.13929202357494219</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9">
+      <c r="G4">
+        <f>G3+0.5</f>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.25918177931828212</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9">
+      <c r="D5" s="24">
+        <v>5.6620000000000008</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.83260000000000001</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G15" si="1">G4+0.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.36237184837822667</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.45118836390597361</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9">
+      <c r="D7" s="25">
+        <v>4.4820000000000002</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.80959999999999999</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.52763344725898531</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.59343034025940078</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.65006225088884473</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9">
+      <c r="D10" s="24">
+        <v>0.79599999999999993</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.2238</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.69880578808779781</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9">
+      <c r="D11" s="24">
+        <v>1.2240000000000002</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.34360000000000002</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.74075973935410844</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0.77686983985157021</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9">
+      <c r="D13" s="24">
+        <v>3.6719999999999997</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.63280000000000003</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0.80795009137924589</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0.83470111177841344</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9">
+      <c r="D15" s="25">
+        <v>3.5200000000000005</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.85772592841348638</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="4:9">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="4:9">
+      <c r="D18" s="24">
+        <v>1.232</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.31379999999999997</v>
+      </c>
+      <c r="G18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9">
+      <c r="D19" s="24">
+        <v>3.1719999999999997</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="G19">
+        <v>0.2</v>
+      </c>
+      <c r="H19">
+        <f>1-EXP(-$I$19*G19)</f>
+        <v>7.1328306158712773E-2</v>
+      </c>
+      <c r="I19">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9">
+      <c r="G20">
+        <v>0.5</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H32" si="2">1-EXP(-$I$19*G20)</f>
+        <v>0.16889571614787435</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9">
+      <c r="D21" s="24">
+        <v>5.74</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G21">
+        <f>G20+0.5</f>
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>0.30926566936264532</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9">
+      <c r="G22">
+        <f t="shared" ref="G22:G32" si="3">G21+0.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>0.42592773880356394</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9">
+      <c r="D23" s="25">
+        <v>3.9899999999999998</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>0.52288608447896556</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>0.6034685809250071</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>0.67044103892481088</v>
+      </c>
+    </row>
+    <row r="26" spans="4:9">
+      <c r="D26" s="24">
+        <v>0.85</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.24500000000000011</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>3.5</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>0.72610213566855442</v>
+      </c>
+    </row>
+    <row r="27" spans="4:9">
+      <c r="D27" s="24">
+        <v>1.1719999999999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.35859999999999992</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>0.77236231161618729</v>
+      </c>
+    </row>
+    <row r="28" spans="4:9">
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>4.5</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>0.81080934201801802</v>
+      </c>
+    </row>
+    <row r="29" spans="4:9">
+      <c r="D29" s="24">
+        <v>4.0600000000000005</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.74560000000000004</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>0.84276283368637239</v>
+      </c>
+    </row>
+    <row r="30" spans="4:9">
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>5.5</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>0.86931951749597491</v>
+      </c>
+    </row>
+    <row r="31" spans="4:9">
+      <c r="D31" s="25">
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.68419999999999992</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>0.891390891175042</v>
+      </c>
+    </row>
+    <row r="32" spans="4:9">
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>0.90973450439021564</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W40"/>
   <sheetViews>
@@ -22707,7 +24818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
@@ -22945,12 +25056,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AF48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD48" sqref="AD48"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="14.35"/>
@@ -24598,7 +26709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C3:F28"/>
   <sheetViews>
@@ -25028,7 +27139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:J37"/>
   <sheetViews>
@@ -25652,7 +27763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
@@ -26433,7 +28544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Change Kun8182 to not harvest till observed date
</commit_message>
<xml_diff>
--- a/Prototypes/Peanut/Observed.xlsx
+++ b/Prototypes/Peanut/Observed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Peanut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBEB05E-8424-483B-BFD0-4F1312734F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AEC314-DB5B-4132-B11A-4885860B9C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="170">
   <si>
     <t>SimulationName</t>
   </si>
@@ -548,6 +548,12 @@
   </si>
   <si>
     <t>Peanut.Pod.HarvestIndex</t>
+  </si>
+  <si>
+    <t>Kunnunura8182Pop9</t>
+  </si>
+  <si>
+    <t>Kunnunura8182Pop27</t>
   </si>
 </sst>
 </file>
@@ -6000,21 +6006,21 @@
   <dimension ref="A1:AC372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8880" ySplit="1428" topLeftCell="C335" activePane="topRight"/>
+      <pane xSplit="8880" ySplit="1425" topLeftCell="C278" activePane="bottomLeft"/>
       <selection pane="topRight" activeCell="AA2" sqref="AA2"/>
-      <selection pane="bottomLeft" activeCell="D320" sqref="D320"/>
+      <selection pane="bottomLeft" activeCell="A308" sqref="A308:A320"/>
       <selection pane="bottomRight" activeCell="AA340" sqref="AA340"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.41015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.52734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.52734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.76171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="72">
+    <row r="1" spans="1:29" ht="57.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -19720,7 +19726,7 @@
     </row>
     <row r="295" spans="1:27">
       <c r="A295" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B295" s="1"/>
       <c r="C295" s="8">
@@ -19762,7 +19768,7 @@
     </row>
     <row r="296" spans="1:27">
       <c r="A296" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B296" s="1"/>
       <c r="C296" s="8">
@@ -19804,7 +19810,7 @@
     </row>
     <row r="297" spans="1:27">
       <c r="A297" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B297" s="1"/>
       <c r="C297" s="8">
@@ -19846,7 +19852,7 @@
     </row>
     <row r="298" spans="1:27">
       <c r="A298" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B298" s="1"/>
       <c r="C298" s="8">
@@ -19888,7 +19894,7 @@
     </row>
     <row r="299" spans="1:27">
       <c r="A299" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B299" s="1"/>
       <c r="C299" s="8">
@@ -19930,7 +19936,7 @@
     </row>
     <row r="300" spans="1:27">
       <c r="A300" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B300" s="1"/>
       <c r="C300" s="8">
@@ -19972,7 +19978,7 @@
     </row>
     <row r="301" spans="1:27">
       <c r="A301" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B301" s="1"/>
       <c r="C301" s="8">
@@ -20014,7 +20020,7 @@
     </row>
     <row r="302" spans="1:27">
       <c r="A302" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B302" s="1"/>
       <c r="C302" s="8">
@@ -20056,7 +20062,7 @@
     </row>
     <row r="303" spans="1:27">
       <c r="A303" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B303" s="1"/>
       <c r="C303" s="8">
@@ -20098,7 +20104,7 @@
     </row>
     <row r="304" spans="1:27">
       <c r="A304" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B304" s="1"/>
       <c r="C304" s="8">
@@ -20140,7 +20146,7 @@
     </row>
     <row r="305" spans="1:27">
       <c r="A305" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B305" s="1"/>
       <c r="C305" s="8">
@@ -20180,7 +20186,7 @@
     </row>
     <row r="306" spans="1:27">
       <c r="A306" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B306" s="1"/>
       <c r="C306" s="8">
@@ -20220,7 +20226,7 @@
     </row>
     <row r="307" spans="1:27">
       <c r="A307" s="1" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="B307" s="1"/>
       <c r="C307" s="8">
@@ -20265,7 +20271,7 @@
     </row>
     <row r="308" spans="1:27">
       <c r="A308" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B308" s="1"/>
       <c r="C308" s="8">
@@ -20307,7 +20313,7 @@
     </row>
     <row r="309" spans="1:27">
       <c r="A309" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B309" s="1"/>
       <c r="C309" s="8">
@@ -20349,7 +20355,7 @@
     </row>
     <row r="310" spans="1:27">
       <c r="A310" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B310" s="1"/>
       <c r="C310" s="8">
@@ -20391,7 +20397,7 @@
     </row>
     <row r="311" spans="1:27">
       <c r="A311" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B311" s="1"/>
       <c r="C311" s="8">
@@ -20433,7 +20439,7 @@
     </row>
     <row r="312" spans="1:27">
       <c r="A312" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B312" s="1"/>
       <c r="C312" s="8">
@@ -20475,7 +20481,7 @@
     </row>
     <row r="313" spans="1:27">
       <c r="A313" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B313" s="1"/>
       <c r="C313" s="8">
@@ -20517,7 +20523,7 @@
     </row>
     <row r="314" spans="1:27">
       <c r="A314" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B314" s="1"/>
       <c r="C314" s="8">
@@ -20559,7 +20565,7 @@
     </row>
     <row r="315" spans="1:27">
       <c r="A315" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B315" s="1"/>
       <c r="C315" s="8">
@@ -20601,7 +20607,7 @@
     </row>
     <row r="316" spans="1:27">
       <c r="A316" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B316" s="1"/>
       <c r="C316" s="8">
@@ -20643,7 +20649,7 @@
     </row>
     <row r="317" spans="1:27">
       <c r="A317" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B317" s="1"/>
       <c r="C317" s="8">
@@ -20685,7 +20691,7 @@
     </row>
     <row r="318" spans="1:27">
       <c r="A318" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B318" s="1"/>
       <c r="C318" s="8">
@@ -20725,7 +20731,7 @@
     </row>
     <row r="319" spans="1:27">
       <c r="A319" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B319" s="1"/>
       <c r="C319" s="8">
@@ -20765,7 +20771,7 @@
     </row>
     <row r="320" spans="1:27">
       <c r="A320" s="1" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B320" s="1"/>
       <c r="C320" s="8">
@@ -23035,7 +23041,7 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <sheetData>
     <row r="1" spans="4:9">
       <c r="D1" t="s">
@@ -23467,7 +23473,7 @@
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="14.35"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="B1" t="s">
@@ -24858,7 +24864,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="14.35"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
@@ -25098,7 +25104,7 @@
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="14.35"/>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1">
@@ -26751,7 +26757,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="14.35"/>
   <sheetData>
     <row r="3" spans="3:6">
       <c r="C3" t="s">
@@ -27181,7 +27187,7 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="14.35"/>
   <sheetData>
     <row r="1" spans="2:9">
       <c r="B1" t="s">
@@ -27805,7 +27811,7 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="14.35"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1">
@@ -28586,9 +28592,9 @@
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.1171875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">

</xml_diff>